<commit_message>
WIP: ForecastExport: month + 1 -> month, debitor invoices added for actual sums.
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F04B54-C5FF-3F48-B44F-F5DD81DA3941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7920505-9CF4-A041-B4BA-26E14C7865AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="36480" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="36480" windowHeight="23540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forecast_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Grafiken" sheetId="2" r:id="rId2"/>
     <sheet name="Umsatz kumuliert" sheetId="3" r:id="rId3"/>
+    <sheet name="Rechnungen" sheetId="4" r:id="rId4"/>
+    <sheet name="Rechnungen Vorjahr" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__xlfn_SUMIFS">#N/A</definedName>
@@ -34,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>Nr.</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
     <t>Angebotsdatum</t>
   </si>
   <si>
@@ -108,12 +107,6 @@
     <t>Wahrscheinlichkeitswert</t>
   </si>
   <si>
-    <t>Monatsende Startdatum +1</t>
-  </si>
-  <si>
-    <t>Monatsende Enddatum +1</t>
-  </si>
-  <si>
     <t>Anzahl Monate</t>
   </si>
   <si>
@@ -190,6 +183,33 @@
   </si>
   <si>
     <t>Kunde</t>
+  </si>
+  <si>
+    <t>Betreff</t>
+  </si>
+  <si>
+    <t>Pos.</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Bezahldatum</t>
+  </si>
+  <si>
+    <t>Netto</t>
+  </si>
+  <si>
+    <t>Auftrag</t>
+  </si>
+  <si>
+    <t>Positionstext</t>
+  </si>
+  <si>
+    <t>Monatsende Startdatum</t>
+  </si>
+  <si>
+    <t>Monatsende Enddatum</t>
   </si>
 </sst>
 </file>
@@ -448,7 +468,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -472,15 +492,9 @@
     <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -495,6 +509,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent 1 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2094,25 +2117,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z9" sqref="Z9"/>
+      <selection pane="bottomRight" activeCell="AQ22" sqref="AQ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" style="26" customWidth="1"/>
-    <col min="6" max="7" width="31.1640625" style="26" customWidth="1"/>
-    <col min="8" max="11" width="11.5" style="26" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" style="22" customWidth="1"/>
+    <col min="6" max="7" width="31.1640625" style="22" customWidth="1"/>
+    <col min="8" max="11" width="11.5" style="22" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" customWidth="1"/>
     <col min="13" max="16" width="11.5" style="2" customWidth="1"/>
-    <col min="17" max="17" width="11.5" style="25" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="21" customWidth="1"/>
     <col min="18" max="19" width="11.5" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.5" customWidth="1"/>
     <col min="21" max="21" width="11.5" style="2" customWidth="1"/>
@@ -2120,143 +2143,143 @@
     <col min="24" max="24" width="8" customWidth="1"/>
     <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
     <col min="26" max="37" width="12.83203125" style="2" customWidth="1"/>
-    <col min="38" max="39" width="19" style="29" customWidth="1"/>
-    <col min="40" max="40" width="11.5" style="26" customWidth="1"/>
-    <col min="41" max="41" width="16.5" style="26" customWidth="1"/>
-    <col min="42" max="42" width="29.5" style="26" customWidth="1"/>
-    <col min="43" max="43" width="65.6640625" style="26" customWidth="1"/>
+    <col min="38" max="39" width="19" style="25" customWidth="1"/>
+    <col min="40" max="40" width="11.5" style="22" customWidth="1"/>
+    <col min="41" max="41" width="16.5" style="22" customWidth="1"/>
+    <col min="42" max="42" width="29.5" style="22" customWidth="1"/>
+    <col min="43" max="43" width="65.6640625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:43" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="S1" s="26"/>
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="U1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Y1" s="3"/>
       <c r="Z1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="AF1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AI1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL1" s="28" t="s">
+      <c r="AL1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="AM1" s="28" t="s">
+      <c r="AN1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AN1" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO1" s="27" t="s">
+      <c r="AO1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AP1" s="27" t="s">
+      <c r="AQ1" s="23" t="s">
         <v>21</v>
-      </c>
-      <c r="AQ1" s="27" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y2" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Z2" s="7">
         <f t="shared" ref="Z2:AK2" si="0">SUMIFS(Z10:Z65537,$K10:$K65537,"=beauftragt")</f>
@@ -2309,313 +2332,325 @@
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y3" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Z3" s="9">
-        <f>SUMIFS(Z10:Z65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" ref="Z3:AK3" si="1">SUMIFS(Z10:Z65537,$K10:$K65537,"=gelegt")</f>
         <v>0</v>
       </c>
       <c r="AA3" s="9">
-        <f>SUMIFS(AA10:AA65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB3" s="9">
-        <f>SUMIFS(AB10:AB65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC3" s="9">
-        <f>SUMIFS(AC10:AC65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD3" s="9">
-        <f>SUMIFS(AD10:AD65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE3" s="9">
-        <f>SUMIFS(AE10:AE65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF3" s="9">
-        <f>SUMIFS(AF10:AF65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG3" s="9">
-        <f>SUMIFS(AG10:AG65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH3" s="9">
-        <f>SUMIFS(AH10:AH65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI3" s="9">
-        <f>SUMIFS(AI10:AI65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="9">
-        <f>SUMIFS(AJ10:AJ65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK3" s="9">
-        <f>SUMIFS(AK10:AK65537,$K10:$K65537,"=gelegt")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y4" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Z4" s="7">
-        <f>SUMIFS(Z10:Z65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" ref="Z4:AK4" si="2">SUMIFS(Z10:Z65537,$K10:$K65537,"=LOI")</f>
         <v>0</v>
       </c>
       <c r="AA4" s="7">
-        <f>SUMIFS(AA10:AA65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB4" s="7">
-        <f>SUMIFS(AB10:AB65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC4" s="7">
-        <f>SUMIFS(AC10:AC65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD4" s="7">
-        <f>SUMIFS(AD10:AD65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE4" s="7">
-        <f>SUMIFS(AE10:AE65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF4" s="7">
-        <f>SUMIFS(AF10:AF65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG4" s="7">
-        <f>SUMIFS(AG10:AG65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH4" s="7">
-        <f>SUMIFS(AH10:AH65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI4" s="7">
-        <f>SUMIFS(AI10:AI65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="7">
-        <f>SUMIFS(AJ10:AJ65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK4" s="7">
-        <f>SUMIFS(AK10:AK65537,$K10:$K65537,"=LOI")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y5" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Z5" s="9">
-        <f>SUMIFS(Z10:Z65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" ref="Z5:AE5" si="3">SUMIFS(Z10:Z65537,$K10:$K65537,"=in Erstellung")</f>
         <v>0</v>
       </c>
       <c r="AA5" s="9">
-        <f>SUMIFS(AA10:AA65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB5" s="9">
-        <f>SUMIFS(AB10:AB65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC5" s="9">
-        <f>SUMIFS(AC10:AC65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD5" s="9">
-        <f>SUMIFS(AD10:AD65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE5" s="9">
-        <f>SUMIFS(AE10:AE65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF5" s="9">
-        <f t="shared" ref="AF5:AK5" si="1">SUMIFS(AF10:AF65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" ref="AF5:AK5" si="4">SUMIFS(AF10:AF65537,$K10:$K65537,"=in Erstellung")</f>
         <v>0</v>
       </c>
       <c r="AG5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AK5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y6" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Z6" s="11">
-        <f t="shared" ref="Z6:AK6" si="2">SUMIFS(Z10:Z65537,$K10:$K65537,"=Potenzial")</f>
+        <f t="shared" ref="Z6:AK6" si="5">SUMIFS(Z10:Z65537,$K10:$K65537,"=Potenzial")</f>
         <v>0</v>
       </c>
       <c r="AA6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AH6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AI6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AK6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y7" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Z7" s="9">
-        <f t="shared" ref="Z7:AK7" si="3">SUM(Z2:Z6)</f>
+        <f t="shared" ref="Z7:AK7" si="6">SUM(Z2:Z6)</f>
         <v>0</v>
       </c>
       <c r="AA7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AH7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AK7" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y8" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Z8" s="14">
+        <f>SUM(Rechnungen!M2:M65535)</f>
         <v>0</v>
       </c>
       <c r="AA8" s="14">
+        <f>SUM(Rechnungen!N2:N65535)</f>
         <v>0</v>
       </c>
       <c r="AB8" s="14">
+        <f>SUM(Rechnungen!O2:O65535)</f>
         <v>0</v>
       </c>
       <c r="AC8" s="14">
+        <f>SUM(Rechnungen!P2:P65535)</f>
         <v>0</v>
       </c>
       <c r="AD8" s="14">
+        <f>SUM(Rechnungen!Q2:Q65535)</f>
         <v>0</v>
       </c>
       <c r="AE8" s="14">
+        <f>SUM(Rechnungen!R2:R65535)</f>
         <v>0</v>
       </c>
       <c r="AF8" s="14">
+        <f>SUM(Rechnungen!S2:S65535)</f>
         <v>0</v>
       </c>
       <c r="AG8" s="14">
+        <f>SUM(Rechnungen!T2:T65535)</f>
         <v>0</v>
       </c>
       <c r="AH8" s="14">
+        <f>SUM(Rechnungen!U2:U65535)</f>
         <v>0</v>
       </c>
       <c r="AI8" s="14">
+        <f>SUM(Rechnungen!V2:V65535)</f>
         <v>0</v>
       </c>
       <c r="AJ8" s="14">
+        <f>SUM(Rechnungen!W2:W65535)</f>
         <v>0</v>
       </c>
       <c r="AK8" s="14">
+        <f>SUM(Rechnungen!X2:X65535)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y9" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Z9" s="16">
         <v>0</v>
@@ -2672,7 +2707,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V57" sqref="V57"/>
     </sheetView>
   </sheetViews>
@@ -2696,336 +2731,337 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="13" width="17" customWidth="1"/>
+    <col min="1" max="1" width="17" style="13" customWidth="1"/>
+    <col min="2" max="13" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B1" s="17" t="str">
+    <row r="1" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="28" t="str">
         <f>Forecast_Data!Z1</f>
         <v>Month 1</v>
       </c>
-      <c r="C1" s="17" t="str">
+      <c r="C1" s="28" t="str">
         <f>Forecast_Data!AA1</f>
         <v>Month 2</v>
       </c>
-      <c r="D1" s="17" t="str">
+      <c r="D1" s="28" t="str">
         <f>Forecast_Data!AB1</f>
         <v>Month 3</v>
       </c>
-      <c r="E1" s="17" t="str">
+      <c r="E1" s="28" t="str">
         <f>Forecast_Data!AC1</f>
         <v>Month 4</v>
       </c>
-      <c r="F1" s="17" t="str">
+      <c r="F1" s="28" t="str">
         <f>Forecast_Data!AD1</f>
         <v>Month 5</v>
       </c>
-      <c r="G1" s="17" t="str">
+      <c r="G1" s="28" t="str">
         <f>Forecast_Data!AE1</f>
         <v>Month 6</v>
       </c>
-      <c r="H1" s="17" t="str">
+      <c r="H1" s="28" t="str">
         <f>Forecast_Data!AF1</f>
         <v>Month 7</v>
       </c>
-      <c r="I1" s="17" t="str">
+      <c r="I1" s="28" t="str">
         <f>Forecast_Data!AG1</f>
         <v>Month 8</v>
       </c>
-      <c r="J1" s="17" t="str">
+      <c r="J1" s="28" t="str">
         <f>Forecast_Data!AH1</f>
         <v>Month 9</v>
       </c>
-      <c r="K1" s="17" t="str">
+      <c r="K1" s="28" t="str">
         <f>Forecast_Data!AI1</f>
         <v>Month 10</v>
       </c>
-      <c r="L1" s="17" t="str">
+      <c r="L1" s="28" t="str">
         <f>Forecast_Data!AJ1</f>
         <v>Month 11</v>
       </c>
-      <c r="M1" s="17" t="str">
+      <c r="M1" s="28" t="str">
         <f>Forecast_Data!AK1</f>
         <v>Month 12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="19">
+      <c r="A2" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="17">
         <f>Forecast_Data!Z8</f>
         <v>0</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="17">
         <f>Forecast_Data!AA8</f>
         <v>0</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="17">
         <f>Forecast_Data!AB8</f>
         <v>0</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="17">
         <f>Forecast_Data!AC8</f>
         <v>0</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="17">
         <f>Forecast_Data!AD8</f>
         <v>0</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="17">
         <f>Forecast_Data!AE8</f>
         <v>0</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="17">
         <f>Forecast_Data!AF8</f>
         <v>0</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="17">
         <f>Forecast_Data!AG8</f>
         <v>0</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="17">
         <f>Forecast_Data!AH8</f>
         <v>0</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="17">
         <f>Forecast_Data!AI8</f>
         <v>0</v>
       </c>
-      <c r="L2" s="19">
+      <c r="L2" s="17">
         <f>Forecast_Data!AJ8</f>
         <v>0</v>
       </c>
-      <c r="M2" s="19">
+      <c r="M2" s="17">
         <f>Forecast_Data!AK8</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="20">
+      <c r="A3" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="18">
         <f>Forecast_Data!Z7</f>
         <v>0</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="18">
         <f>Forecast_Data!AA7</f>
         <v>0</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="18">
         <f>Forecast_Data!AB7</f>
         <v>0</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="18">
         <f>Forecast_Data!AC7</f>
         <v>0</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="18">
         <f>Forecast_Data!AD7</f>
         <v>0</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="18">
         <f>Forecast_Data!AE7</f>
         <v>0</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="18">
         <f>Forecast_Data!AF7</f>
         <v>0</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="18">
         <f>Forecast_Data!AG7</f>
         <v>0</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="18">
         <f>Forecast_Data!AH7</f>
         <v>0</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="18">
         <f>Forecast_Data!AI7</f>
         <v>0</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="18">
         <f>Forecast_Data!AJ7</f>
         <v>0</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="18">
         <f>Forecast_Data!AK7</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="20">
+      <c r="A4" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="18">
         <f t="shared" ref="B4:M4" si="0">IF(B2 &gt; 0,B2,B3)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="22">
+      <c r="A5" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="19">
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="19">
         <f>B5+C4</f>
         <v>0</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="19">
         <f t="shared" ref="D5:M5" si="1">C5+D4</f>
         <v>0</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="22">
+      <c r="A6" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="19">
         <f>Forecast_Data!Z9</f>
         <v>0</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="19">
         <f>B6+Forecast_Data!AA9</f>
         <v>0</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="19">
         <f>C6+Forecast_Data!AB9</f>
         <v>0</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="19">
         <f>D6+Forecast_Data!AC9</f>
         <v>0</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="19">
         <f>E6+Forecast_Data!AD9</f>
         <v>0</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="19">
         <f>F6+Forecast_Data!AE9</f>
         <v>0</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="19">
         <f>G6+Forecast_Data!AF9</f>
         <v>0</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="19">
         <f>H6+Forecast_Data!AG9</f>
         <v>0</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="19">
         <f>I6+Forecast_Data!AH9</f>
         <v>0</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="19">
         <f>J6+Forecast_Data!AI9</f>
         <v>0</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="19">
         <f>K6+Forecast_Data!AJ9</f>
         <v>0</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="19">
         <f>L6+Forecast_Data!AK9</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3033,4 +3069,203 @@
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFD20-C3FD-B945-8889-0EABEB8C212C}">
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="27"/>
+      <c r="K1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477A8465-810E-0B43-A1C7-F27798459BF0}">
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="27"/>
+      <c r="K1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ForecastExport shows now all invoices (also from previous year).
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7920505-9CF4-A041-B4BA-26E14C7865AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B54E4E1-762A-9842-9954-998FFFBE480E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="36480" windowHeight="23540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>Nr.</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Monatsende Enddatum</t>
+  </si>
+  <si>
+    <t>Vorjahr</t>
   </si>
 </sst>
 </file>
@@ -509,15 +512,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent 1 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2118,10 +2121,10 @@
   <dimension ref="A1:AQ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ22" sqref="AQ22"/>
+      <selection pane="bottomRight" activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2202,10 +2205,10 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="26"/>
+      <c r="S1" s="29"/>
       <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
@@ -2723,10 +2726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2736,57 +2739,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="28" t="str">
+      <c r="B1" s="26" t="str">
         <f>Forecast_Data!Z1</f>
         <v>Month 1</v>
       </c>
-      <c r="C1" s="28" t="str">
+      <c r="C1" s="26" t="str">
         <f>Forecast_Data!AA1</f>
         <v>Month 2</v>
       </c>
-      <c r="D1" s="28" t="str">
+      <c r="D1" s="26" t="str">
         <f>Forecast_Data!AB1</f>
         <v>Month 3</v>
       </c>
-      <c r="E1" s="28" t="str">
+      <c r="E1" s="26" t="str">
         <f>Forecast_Data!AC1</f>
         <v>Month 4</v>
       </c>
-      <c r="F1" s="28" t="str">
+      <c r="F1" s="26" t="str">
         <f>Forecast_Data!AD1</f>
         <v>Month 5</v>
       </c>
-      <c r="G1" s="28" t="str">
+      <c r="G1" s="26" t="str">
         <f>Forecast_Data!AE1</f>
         <v>Month 6</v>
       </c>
-      <c r="H1" s="28" t="str">
+      <c r="H1" s="26" t="str">
         <f>Forecast_Data!AF1</f>
         <v>Month 7</v>
       </c>
-      <c r="I1" s="28" t="str">
+      <c r="I1" s="26" t="str">
         <f>Forecast_Data!AG1</f>
         <v>Month 8</v>
       </c>
-      <c r="J1" s="28" t="str">
+      <c r="J1" s="26" t="str">
         <f>Forecast_Data!AH1</f>
         <v>Month 9</v>
       </c>
-      <c r="K1" s="28" t="str">
+      <c r="K1" s="26" t="str">
         <f>Forecast_Data!AI1</f>
         <v>Month 10</v>
       </c>
-      <c r="L1" s="28" t="str">
+      <c r="L1" s="26" t="str">
         <f>Forecast_Data!AJ1</f>
         <v>Month 11</v>
       </c>
-      <c r="M1" s="28" t="str">
+      <c r="M1" s="26" t="str">
         <f>Forecast_Data!AK1</f>
         <v>Month 12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="17">
@@ -2839,7 +2842,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="18">
@@ -2892,7 +2895,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="27" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="18">
@@ -2945,7 +2948,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="19">
@@ -2998,7 +3001,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="19">
@@ -3062,6 +3065,59 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!M2:M65534)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!N2:N65534)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!O2:O65534)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!P2:P65534)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!Q2:Q65534)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!R2:R65534)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!S2:S65534)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!T2:T65534)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!U2:U65534)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!V2:V65534)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!W2:W65534)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="19">
+        <f>SUM('Rechnungen Vorjahr'!X2:X65534)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3079,7 +3135,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3115,10 +3171,10 @@
       <c r="H1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="27"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="13" t="s">
         <v>54</v>
       </c>
@@ -3179,7 +3235,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3215,10 +3271,10 @@
       <c r="H1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="27"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="13" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
WIP: ForecastExport should work for now...
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA02478F-6E6D-E04F-9E09-6C7C301786C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1FE72E-2B8D-4344-AFAE-2244A645A354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="460" windowWidth="36480" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="36480" windowHeight="23540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forecast_Data" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; €&quot;"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -343,12 +343,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -564,16 +558,16 @@
     <xf numFmtId="49" fontId="12" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent 1 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2145,7 +2139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2169,7 +2163,7 @@
     <col min="21" max="21" width="11.5" style="2" customWidth="1"/>
     <col min="22" max="23" width="14" style="1" customWidth="1"/>
     <col min="24" max="24" width="8" customWidth="1"/>
-    <col min="25" max="25" width="11.5" style="34" customWidth="1"/>
+    <col min="25" max="25" width="11.5" style="32" customWidth="1"/>
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
     <col min="27" max="38" width="12.83203125" style="2" customWidth="1"/>
     <col min="39" max="40" width="19" style="25" customWidth="1"/>
@@ -2232,10 +2226,10 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="31"/>
+      <c r="S1" s="33"/>
       <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
@@ -2251,7 +2245,7 @@
       <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Y1" s="31" t="s">
         <v>61</v>
       </c>
       <c r="Z1" s="3"/>
@@ -2744,7 +2738,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
@@ -3256,10 +3250,10 @@
       <c r="H1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="32"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="13" t="s">
         <v>54</v>
       </c>
@@ -3356,10 +3350,10 @@
       <c r="H1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="32"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="13" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
ForecastTemplate: Info about probabilities added as new sheet.
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CD398A-CC85-9C4C-9FEF-784CD8EB1B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683F4FAB-4D2C-2041-A0EF-005D1835AE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="36480" windowHeight="23540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Umsatz kumuliert" sheetId="3" r:id="rId3"/>
     <sheet name="Rechnungen" sheetId="4" r:id="rId4"/>
     <sheet name="Rechnungen Vorjahr" sheetId="6" r:id="rId5"/>
+    <sheet name="Info" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="__xlfn_SUMIFS">#N/A</definedName>
@@ -28,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -72,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="75">
   <si>
     <t>Nr.</t>
   </si>
@@ -252,6 +255,53 @@
   </si>
   <si>
     <t>HOB</t>
+  </si>
+  <si>
+    <t>Auftragsstatus</t>
+  </si>
+  <si>
+    <t>Positionsstatus</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>ABGELEHNT</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>ERSETZT</t>
+  </si>
+  <si>
+    <t>POTENZIAL</t>
+  </si>
+  <si>
+    <t>or value</t>
+  </si>
+  <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
+    <t>BEAUFTRAGT</t>
+  </si>
+  <si>
+    <t>ABGESCHLOSSEN</t>
+  </si>
+  <si>
+    <t>ESKALATION, GELEGT, IN_ERSTELLUNG</t>
+  </si>
+  <si>
+    <t>ESKALATION, GELEGT, IN_ERSTELLUNG, LOI</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>The probability of an order (position) is determined by the following steps (beginning with step 1).
+The first matching entry is used. 'or value' means, that the probaility value given in the order is used, if given,
+otherwise the default probability value is assumed.</t>
   </si>
 </sst>
 </file>
@@ -264,7 +314,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; €&quot;"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -356,6 +406,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -522,7 +580,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -574,11 +632,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -2249,10 +2311,10 @@
       <c r="S1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="33"/>
+      <c r="U1" s="34"/>
       <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
@@ -2749,7 +2811,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
@@ -3261,10 +3325,10 @@
       <c r="H1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="34"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="13" t="s">
         <v>51</v>
       </c>
@@ -3361,10 +3425,10 @@
       <c r="H1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="34"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="13" t="s">
         <v>51</v>
       </c>
@@ -3414,4 +3478,265 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB315FBD-69C9-F248-8D6C-0E7BAAF44D90}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16">
+        <v>0.9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hint added to ForecastTemplate.
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB440B7D-5A19-314D-8E17-CC8A101350CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D912229-6680-DB4C-BDAF-C2145AE97B49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="36480" windowHeight="23540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,10 +21,6 @@
     <sheet name="Rechnungen Vorjahr" sheetId="6" r:id="rId6"/>
     <sheet name="Info" sheetId="7" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__xlfn_SUMIFS">#N/A</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AJ$9</definedName>
@@ -1891,7 +1887,7 @@
             <c:numRef>
               <c:f>'Umsatz kumuliert'!$B$5:$M$5</c:f>
               <c:numCache>
-                <c:formatCode>#.##000" €"</c:formatCode>
+                <c:formatCode>#,##0.00" €"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2260,7 +2256,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#.##000&quot; €&quot;" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2582,7 +2578,7 @@
             <c:numRef>
               <c:f>'Umsatz kumuliert'!$B$5:$M$5</c:f>
               <c:numCache>
-                <c:formatCode>#.##000" €"</c:formatCode>
+                <c:formatCode>#,##0.00" €"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3099,7 +3095,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#.##000&quot; €&quot;" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5870,6 +5866,103 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Textfeld 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97D60B30-C0AF-E040-A430-75769E8C30E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10604500" y="6565900"/>
+          <a:ext cx="3162300" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Anmerkung:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Die IST-Daten im aktuellen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Monat dienen nur der Information und dürfen nicht dem Monatsprognosewert hinzugefügt werden!</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5952,666 +6045,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Forecast_Data"/>
-      <sheetName val="Grafiken"/>
-      <sheetName val="Umsatz kumuliert"/>
-      <sheetName val="Rechnungen"/>
-      <sheetName val="Rechnungen Vorjahr"/>
-      <sheetName val="Info"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="Y1" t="str">
-            <v>Mai 2020</v>
-          </cell>
-          <cell r="Z1" t="str">
-            <v>Jun 2020</v>
-          </cell>
-          <cell r="AA1" t="str">
-            <v>Jul 2020</v>
-          </cell>
-          <cell r="AB1" t="str">
-            <v>Aug 2020</v>
-          </cell>
-          <cell r="AC1" t="str">
-            <v>Sep 2020</v>
-          </cell>
-          <cell r="AD1" t="str">
-            <v>Okt 2020</v>
-          </cell>
-          <cell r="AE1" t="str">
-            <v>Nov 2020</v>
-          </cell>
-          <cell r="AF1" t="str">
-            <v>Dez 2020</v>
-          </cell>
-          <cell r="AG1" t="str">
-            <v>Jan 2021</v>
-          </cell>
-          <cell r="AH1" t="str">
-            <v>Feb 2021</v>
-          </cell>
-          <cell r="AI1" t="str">
-            <v>Mär 2021</v>
-          </cell>
-          <cell r="AJ1" t="str">
-            <v>Apr 2021</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="Y2">
-            <v>627214.2300000001</v>
-          </cell>
-          <cell r="Z2">
-            <v>988250.19</v>
-          </cell>
-          <cell r="AA2">
-            <v>943692.81999999983</v>
-          </cell>
-          <cell r="AB2">
-            <v>602489.71000000008</v>
-          </cell>
-          <cell r="AC2">
-            <v>626160.51000000013</v>
-          </cell>
-          <cell r="AD2">
-            <v>325130.30000000005</v>
-          </cell>
-          <cell r="AE2">
-            <v>362281.76</v>
-          </cell>
-          <cell r="AF2">
-            <v>347671.05000000005</v>
-          </cell>
-          <cell r="AG2">
-            <v>828132.45000000007</v>
-          </cell>
-          <cell r="AH2">
-            <v>9225</v>
-          </cell>
-          <cell r="AI2">
-            <v>9225</v>
-          </cell>
-          <cell r="AJ2">
-            <v>465011.4</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="Y3">
-            <v>80521.34</v>
-          </cell>
-          <cell r="Z3">
-            <v>136900.35</v>
-          </cell>
-          <cell r="AA3">
-            <v>42364.229999999996</v>
-          </cell>
-          <cell r="AB3">
-            <v>54864.443999999996</v>
-          </cell>
-          <cell r="AC3">
-            <v>160534.59399999998</v>
-          </cell>
-          <cell r="AD3">
-            <v>36599.4</v>
-          </cell>
-          <cell r="AE3">
-            <v>29638.82</v>
-          </cell>
-          <cell r="AF3">
-            <v>22318.82</v>
-          </cell>
-          <cell r="AG3">
-            <v>434536.42</v>
-          </cell>
-          <cell r="AH3">
-            <v>36850.903299999998</v>
-          </cell>
-          <cell r="AI3">
-            <v>36850.903299999998</v>
-          </cell>
-          <cell r="AJ3">
-            <v>36850.903299999998</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="Y4">
-            <v>0</v>
-          </cell>
-          <cell r="Z4">
-            <v>0</v>
-          </cell>
-          <cell r="AA4">
-            <v>0</v>
-          </cell>
-          <cell r="AB4">
-            <v>0</v>
-          </cell>
-          <cell r="AC4">
-            <v>0</v>
-          </cell>
-          <cell r="AD4">
-            <v>0</v>
-          </cell>
-          <cell r="AE4">
-            <v>0</v>
-          </cell>
-          <cell r="AF4">
-            <v>0</v>
-          </cell>
-          <cell r="AG4">
-            <v>0</v>
-          </cell>
-          <cell r="AH4">
-            <v>16419</v>
-          </cell>
-          <cell r="AI4">
-            <v>16419</v>
-          </cell>
-          <cell r="AJ4">
-            <v>16419</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="Y5">
-            <v>900</v>
-          </cell>
-          <cell r="Z5">
-            <v>3786</v>
-          </cell>
-          <cell r="AA5">
-            <v>900</v>
-          </cell>
-          <cell r="AB5">
-            <v>900</v>
-          </cell>
-          <cell r="AC5">
-            <v>30302.68</v>
-          </cell>
-          <cell r="AD5">
-            <v>900</v>
-          </cell>
-          <cell r="AE5">
-            <v>900</v>
-          </cell>
-          <cell r="AF5">
-            <v>900</v>
-          </cell>
-          <cell r="AG5">
-            <v>900</v>
-          </cell>
-          <cell r="AH5">
-            <v>0</v>
-          </cell>
-          <cell r="AI5">
-            <v>0</v>
-          </cell>
-          <cell r="AJ5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="Y6">
-            <v>97492.332899999994</v>
-          </cell>
-          <cell r="Z6">
-            <v>130084.66619999999</v>
-          </cell>
-          <cell r="AA6">
-            <v>226481.33290000001</v>
-          </cell>
-          <cell r="AB6">
-            <v>288304.24950000003</v>
-          </cell>
-          <cell r="AC6">
-            <v>212688.99309999999</v>
-          </cell>
-          <cell r="AD6">
-            <v>153455.82639999999</v>
-          </cell>
-          <cell r="AE6">
-            <v>302595.05909999995</v>
-          </cell>
-          <cell r="AF6">
-            <v>176755.05909999998</v>
-          </cell>
-          <cell r="AG6">
-            <v>195995.05909999998</v>
-          </cell>
-          <cell r="AH6">
-            <v>81088.942299999995</v>
-          </cell>
-          <cell r="AI6">
-            <v>92588.942299999995</v>
-          </cell>
-          <cell r="AJ6">
-            <v>200522.32689999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="Y8">
-            <v>83289.490000000005</v>
-          </cell>
-          <cell r="Z8">
-            <v>0</v>
-          </cell>
-          <cell r="AA8">
-            <v>0</v>
-          </cell>
-          <cell r="AB8">
-            <v>0</v>
-          </cell>
-          <cell r="AC8">
-            <v>0</v>
-          </cell>
-          <cell r="AD8">
-            <v>0</v>
-          </cell>
-          <cell r="AE8">
-            <v>0</v>
-          </cell>
-          <cell r="AF8">
-            <v>0</v>
-          </cell>
-          <cell r="AG8">
-            <v>0</v>
-          </cell>
-          <cell r="AH8">
-            <v>0</v>
-          </cell>
-          <cell r="AI8">
-            <v>0</v>
-          </cell>
-          <cell r="AJ8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="X9" t="str">
-            <v>PLAN</v>
-          </cell>
-          <cell r="Y9">
-            <v>1184124.6616666666</v>
-          </cell>
-          <cell r="Z9">
-            <v>1184124.6616666666</v>
-          </cell>
-          <cell r="AA9">
-            <v>1413179.1716666666</v>
-          </cell>
-          <cell r="AB9">
-            <v>1413179.1716666666</v>
-          </cell>
-          <cell r="AC9">
-            <v>1413179.1716666666</v>
-          </cell>
-          <cell r="AD9">
-            <v>1164681.0383333333</v>
-          </cell>
-          <cell r="AE9">
-            <v>1164681.0383333333</v>
-          </cell>
-          <cell r="AF9">
-            <v>1164681.0383333333</v>
-          </cell>
-          <cell r="AG9">
-            <v>0</v>
-          </cell>
-          <cell r="AH9">
-            <v>0</v>
-          </cell>
-          <cell r="AI9">
-            <v>0</v>
-          </cell>
-          <cell r="AJ9">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Mai 2020</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Jun 2020</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Jul 2020</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>Aug 2020</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>Sep 2020</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>Okt 2020</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>Nov 2020</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>Dez 2020</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>Jan 2021</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>Feb 2021</v>
-          </cell>
-          <cell r="L1" t="str">
-            <v>Mär 2021</v>
-          </cell>
-          <cell r="M1" t="str">
-            <v>Apr 2021</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>889417.39290000009</v>
-          </cell>
-          <cell r="C5">
-            <v>2148438.5991000002</v>
-          </cell>
-          <cell r="D5">
-            <v>3361876.9819999998</v>
-          </cell>
-          <cell r="E5">
-            <v>4308435.3854999999</v>
-          </cell>
-          <cell r="F5">
-            <v>5338122.1625999995</v>
-          </cell>
-          <cell r="G5">
-            <v>5854207.6889999993</v>
-          </cell>
-          <cell r="H5">
-            <v>6549623.3280999996</v>
-          </cell>
-          <cell r="I5">
-            <v>7097268.2571999999</v>
-          </cell>
-          <cell r="J5">
-            <v>8556832.1863000002</v>
-          </cell>
-          <cell r="K5">
-            <v>8700416.0318999998</v>
-          </cell>
-          <cell r="L5">
-            <v>8855499.8774999995</v>
-          </cell>
-          <cell r="M5">
-            <v>9574303.5077</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>1184124.6616666666</v>
-          </cell>
-          <cell r="C6">
-            <v>2368249.3233333332</v>
-          </cell>
-          <cell r="D6">
-            <v>3781428.4950000001</v>
-          </cell>
-          <cell r="E6">
-            <v>5194607.666666667</v>
-          </cell>
-          <cell r="F6">
-            <v>6607786.8383333338</v>
-          </cell>
-          <cell r="G6">
-            <v>7772467.8766666669</v>
-          </cell>
-          <cell r="H6">
-            <v>8937148.915000001</v>
-          </cell>
-          <cell r="I6">
-            <v>10101829.953333335</v>
-          </cell>
-          <cell r="J6">
-            <v>10101829.953333335</v>
-          </cell>
-          <cell r="K6">
-            <v>10101829.953333335</v>
-          </cell>
-          <cell r="L6">
-            <v>10101829.953333335</v>
-          </cell>
-          <cell r="M6">
-            <v>10101829.953333335</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>720137.78999999992</v>
-          </cell>
-          <cell r="C9">
-            <v>1581628.95</v>
-          </cell>
-          <cell r="D9">
-            <v>2801043.7124999994</v>
-          </cell>
-          <cell r="E9">
-            <v>4347637.7249999996</v>
-          </cell>
-          <cell r="F9">
-            <v>5365372.7649999997</v>
-          </cell>
-          <cell r="G9">
-            <v>7029524.5774999997</v>
-          </cell>
-          <cell r="H9">
-            <v>7775036.7299999995</v>
-          </cell>
-          <cell r="I9">
-            <v>10132308.942500001</v>
-          </cell>
-          <cell r="J9">
-            <v>10424002.0625</v>
-          </cell>
-          <cell r="K9">
-            <v>11135444.0075</v>
-          </cell>
-          <cell r="L9">
-            <v>12479049.9025</v>
-          </cell>
-          <cell r="M9">
-            <v>13284954.502499999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Forecast_Data"/>
-      <sheetName val="Grafiken"/>
-      <sheetName val="Umsatz kumuliert"/>
-      <sheetName val="Rechnungen"/>
-      <sheetName val="Rechnungen Vorjahr"/>
-      <sheetName val="Info"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Nov 2019</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Dez 2019</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Jan 2020</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>Feb 2020</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>Mär 2020</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>Apr 2020</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>Mai 2020</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>Jun 2020</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>Jul 2020</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>Aug 2020</v>
-          </cell>
-          <cell r="L1" t="str">
-            <v>Sep 2020</v>
-          </cell>
-          <cell r="M1" t="str">
-            <v>Okt 2020</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>745714.45250000001</v>
-          </cell>
-          <cell r="C5">
-            <v>3102986.6650000014</v>
-          </cell>
-          <cell r="D5">
-            <v>3394679.7850000015</v>
-          </cell>
-          <cell r="E5">
-            <v>4106121.7300000014</v>
-          </cell>
-          <cell r="F5">
-            <v>5449727.6250000019</v>
-          </cell>
-          <cell r="G5">
-            <v>6255632.2250000015</v>
-          </cell>
-          <cell r="H5">
-            <v>7061760.1279000016</v>
-          </cell>
-          <cell r="I5">
-            <v>8320781.3341000015</v>
-          </cell>
-          <cell r="J5">
-            <v>9534219.717000002</v>
-          </cell>
-          <cell r="K5">
-            <v>10480778.120500002</v>
-          </cell>
-          <cell r="L5">
-            <v>11510464.897600003</v>
-          </cell>
-          <cell r="M5">
-            <v>12026550.424000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>1118157.5233333299</v>
-          </cell>
-          <cell r="C6">
-            <v>2236315.0466666599</v>
-          </cell>
-          <cell r="D6">
-            <v>3287213.2383333268</v>
-          </cell>
-          <cell r="E6">
-            <v>4338111.4299999932</v>
-          </cell>
-          <cell r="F6">
-            <v>5389009.6216666596</v>
-          </cell>
-          <cell r="G6">
-            <v>6573134.2833333258</v>
-          </cell>
-          <cell r="H6">
-            <v>7757258.9449999928</v>
-          </cell>
-          <cell r="I6">
-            <v>8941383.6066666599</v>
-          </cell>
-          <cell r="J6">
-            <v>10354562.778333327</v>
-          </cell>
-          <cell r="K6">
-            <v>11767741.949999994</v>
-          </cell>
-          <cell r="L6">
-            <v>13180921.121666661</v>
-          </cell>
-          <cell r="M6">
-            <v>14345602.159999995</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>919174.83499999996</v>
-          </cell>
-          <cell r="C9">
-            <v>3442395.1349999979</v>
-          </cell>
-          <cell r="D9">
-            <v>3652735.2249999978</v>
-          </cell>
-          <cell r="E9">
-            <v>4256051.8124999972</v>
-          </cell>
-          <cell r="F9">
-            <v>4980528.2724999972</v>
-          </cell>
-          <cell r="G9">
-            <v>6283380.3699999973</v>
-          </cell>
-          <cell r="H9">
-            <v>6985012.0349999974</v>
-          </cell>
-          <cell r="I9">
-            <v>7846553.7699999977</v>
-          </cell>
-          <cell r="J9">
-            <v>9066246.6949999966</v>
-          </cell>
-          <cell r="K9">
-            <v>10612992.432499997</v>
-          </cell>
-          <cell r="L9">
-            <v>11630727.472499996</v>
-          </cell>
-          <cell r="M9">
-            <v>13295233.309999997</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7787,7 +7220,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="18">
-        <f t="shared" ref="B4:M4" si="0">IF(B2 &gt; 0,B2,B3)</f>
+        <f t="shared" ref="B4" si="0">IF(B2 &gt; 0,B2,B3)</f>
         <v>0</v>
       </c>
       <c r="C4" s="18">

</xml_diff>

<commit_message>
WIP: order forecast and snapshots.
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E127F8AD-3DF9-8342-8F03-3AFC0DA468D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCB42BB-1B4C-7046-A58B-203456D2D3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="__xlfn_SUMIFS">#N/A</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AK$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AL$9</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t>Nr.</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>Rest</t>
+  </si>
+  <si>
+    <t>Warnung</t>
   </si>
 </sst>
 </file>
@@ -921,7 +924,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$2:$AK$2</c:f>
+              <c:f>Forecast_Data!$AA$2:$AL$2</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1010,7 +1013,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$4:$AK$4</c:f>
+              <c:f>Forecast_Data!$AA$4:$AL$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1099,7 +1102,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$3:$AK$3</c:f>
+              <c:f>Forecast_Data!$AA$3:$AL$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1188,7 +1191,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$6:$AK$6</c:f>
+              <c:f>Forecast_Data!$AA$6:$AL$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1279,7 +1282,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$5:$AK$5</c:f>
+              <c:f>Forecast_Data!$AA$5:$AL$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1354,7 +1357,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$8:$AK$8</c:f>
+              <c:f>Forecast_Data!$AA$8:$AL$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1424,7 +1427,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Forecast_Data!$Y$9</c:f>
+              <c:f>Forecast_Data!$Z$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1453,7 +1456,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Forecast_Data!$Z$1:$AK$1</c:f>
+              <c:f>Forecast_Data!$AA$1:$AL$1</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1497,7 +1500,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$9:$AK$9</c:f>
+              <c:f>Forecast_Data!$AA$9:$AL$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2791,7 +2794,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Forecast_Data!$Y$9</c:f>
+              <c:f>Forecast_Data!$Z$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2823,7 +2826,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$Z$9:$AK$9</c:f>
+              <c:f>Forecast_Data!$AA$9:$AL$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5301,13 +5304,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ9"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5329,16 +5332,17 @@
     <col min="22" max="22" width="8" customWidth="1"/>
     <col min="23" max="23" width="13.33203125" style="25" customWidth="1"/>
     <col min="24" max="24" width="13.1640625" style="25" customWidth="1"/>
-    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="37" width="12.83203125" style="2" customWidth="1"/>
-    <col min="38" max="39" width="19" style="1" customWidth="1"/>
-    <col min="40" max="40" width="52.83203125" customWidth="1"/>
-    <col min="41" max="41" width="16.5" customWidth="1"/>
-    <col min="42" max="42" width="29.5" customWidth="1"/>
-    <col min="43" max="43" width="65.6640625" customWidth="1"/>
+    <col min="25" max="25" width="11.5" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="38" width="12.83203125" style="2" customWidth="1"/>
+    <col min="39" max="40" width="19" style="1" customWidth="1"/>
+    <col min="41" max="41" width="52.83203125" customWidth="1"/>
+    <col min="42" max="42" width="16.5" customWidth="1"/>
+    <col min="43" max="43" width="29.5" customWidth="1"/>
+    <col min="44" max="44" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:44" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5409,72 +5413,71 @@
       <c r="X1" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="22" t="s">
+      <c r="AM1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AM1" s="22" t="s">
+      <c r="AN1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AN1" s="26" t="s">
+      <c r="AO1" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AO1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y2" s="6" t="s">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="7">
-        <f t="shared" ref="Z2:AK2" si="0">SUMIFS(Z10:Z65537,$K10:$K65537,"=beauftragt")</f>
-        <v>0</v>
-      </c>
       <c r="AA2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AA2:AL2" si="0">SUMIFS(AA10:AA65537,$K10:$K65537,"=beauftragt")</f>
         <v>0</v>
       </c>
       <c r="AB2" s="7">
@@ -5517,17 +5520,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AL2" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y3" s="8" t="s">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="9">
-        <f t="shared" ref="Z3:AK3" si="1">SUMIFS(Z10:Z65537,$K10:$K65537,"=gelegt")</f>
-        <v>0</v>
-      </c>
       <c r="AA3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AA3:AL3" si="1">SUMIFS(AA10:AA65537,$K10:$K65537,"=gelegt")</f>
         <v>0</v>
       </c>
       <c r="AB3" s="9">
@@ -5570,17 +5573,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AL3" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y4" s="6" t="s">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z4" s="7">
-        <f t="shared" ref="Z4:AK4" si="2">SUMIFS(Z10:Z65537,$K10:$K65537,"=LOI")</f>
-        <v>0</v>
-      </c>
       <c r="AA4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AA4:AL4" si="2">SUMIFS(AA10:AA65537,$K10:$K65537,"=LOI")</f>
         <v>0</v>
       </c>
       <c r="AB4" s="7">
@@ -5623,17 +5626,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AL4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y5" s="8" t="s">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="Z5" s="9">
-        <f t="shared" ref="Z5:AE5" si="3">SUMIFS(Z10:Z65537,$K10:$K65537,"=in Erstellung")</f>
-        <v>0</v>
-      </c>
       <c r="AA5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AA5:AF5" si="3">SUMIFS(AA10:AA65537,$K10:$K65537,"=in Erstellung")</f>
         <v>0</v>
       </c>
       <c r="AB5" s="9">
@@ -5653,11 +5656,11 @@
         <v>0</v>
       </c>
       <c r="AF5" s="9">
-        <f t="shared" ref="AF5:AK5" si="4">SUMIFS(AF10:AF65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG5" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AG5:AL5" si="4">SUMIFS(AG10:AG65537,$K10:$K65537,"=in Erstellung")</f>
         <v>0</v>
       </c>
       <c r="AH5" s="9">
@@ -5676,17 +5679,17 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="AL5" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y6" s="10" t="s">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="11">
-        <f t="shared" ref="Z6:AK6" si="5">SUMIFS(Z10:Z65537,$K10:$K65537,"=Potenzial")</f>
-        <v>0</v>
-      </c>
       <c r="AA6" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AA6:AL6" si="5">SUMIFS(AA10:AA65537,$K10:$K65537,"=Potenzial")</f>
         <v>0</v>
       </c>
       <c r="AB6" s="11">
@@ -5729,17 +5732,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="AL6" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y7" s="12" t="s">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="Z7" s="9">
-        <f t="shared" ref="Z7:AK7" si="6">SUM(Z2:Z6)</f>
-        <v>0</v>
-      </c>
       <c r="AA7" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AA7:AL7" si="6">SUM(AA2:AA6)</f>
         <v>0</v>
       </c>
       <c r="AB7" s="9">
@@ -5782,67 +5785,68 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AL7" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y8" s="13" t="s">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="Z8" s="14">
+      <c r="AA8" s="14">
         <f>SUM(Rechnungen!M2:M65535)</f>
         <v>0</v>
       </c>
-      <c r="AA8" s="14">
+      <c r="AB8" s="14">
         <f>SUM(Rechnungen!N2:N65535)</f>
         <v>0</v>
       </c>
-      <c r="AB8" s="14">
+      <c r="AC8" s="14">
         <f>SUM(Rechnungen!O2:O65535)</f>
         <v>0</v>
       </c>
-      <c r="AC8" s="14">
+      <c r="AD8" s="14">
         <f>SUM(Rechnungen!P2:P65535)</f>
         <v>0</v>
       </c>
-      <c r="AD8" s="14">
+      <c r="AE8" s="14">
         <f>SUM(Rechnungen!Q2:Q65535)</f>
         <v>0</v>
       </c>
-      <c r="AE8" s="14">
+      <c r="AF8" s="14">
         <f>SUM(Rechnungen!R2:R65535)</f>
         <v>0</v>
       </c>
-      <c r="AF8" s="14">
+      <c r="AG8" s="14">
         <f>SUM(Rechnungen!S2:S65535)</f>
         <v>0</v>
       </c>
-      <c r="AG8" s="14">
+      <c r="AH8" s="14">
         <f>SUM(Rechnungen!T2:T65535)</f>
         <v>0</v>
       </c>
-      <c r="AH8" s="14">
+      <c r="AI8" s="14">
         <f>SUM(Rechnungen!U2:U65535)</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="14">
+      <c r="AJ8" s="14">
         <f>SUM(Rechnungen!V2:V65535)</f>
         <v>0</v>
       </c>
-      <c r="AJ8" s="14">
+      <c r="AK8" s="14">
         <f>SUM(Rechnungen!W2:W65535)</f>
         <v>0</v>
       </c>
-      <c r="AK8" s="14">
+      <c r="AL8" s="14">
         <f>SUM(Rechnungen!X2:X65535)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.15">
-      <c r="Y9" s="15" t="s">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="Z9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="Z9" s="16">
-        <v>0</v>
-      </c>
       <c r="AA9" s="16">
         <v>0</v>
       </c>
@@ -5874,6 +5878,9 @@
         <v>0</v>
       </c>
       <c r="AK9" s="16">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="16">
         <v>0</v>
       </c>
     </row>
@@ -5950,51 +5957,51 @@
   <sheetData>
     <row r="1" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B1" s="23" t="str">
-        <f>Forecast_Data!Z1</f>
+        <f>Forecast_Data!AA1</f>
         <v>Month 1</v>
       </c>
       <c r="C1" s="23" t="str">
-        <f>Forecast_Data!AA1</f>
+        <f>Forecast_Data!AB1</f>
         <v>Month 2</v>
       </c>
       <c r="D1" s="23" t="str">
-        <f>Forecast_Data!AB1</f>
+        <f>Forecast_Data!AC1</f>
         <v>Month 3</v>
       </c>
       <c r="E1" s="23" t="str">
-        <f>Forecast_Data!AC1</f>
+        <f>Forecast_Data!AD1</f>
         <v>Month 4</v>
       </c>
       <c r="F1" s="23" t="str">
-        <f>Forecast_Data!AD1</f>
+        <f>Forecast_Data!AE1</f>
         <v>Month 5</v>
       </c>
       <c r="G1" s="23" t="str">
-        <f>Forecast_Data!AE1</f>
+        <f>Forecast_Data!AF1</f>
         <v>Month 6</v>
       </c>
       <c r="H1" s="23" t="str">
-        <f>Forecast_Data!AF1</f>
+        <f>Forecast_Data!AG1</f>
         <v>Month 7</v>
       </c>
       <c r="I1" s="23" t="str">
-        <f>Forecast_Data!AG1</f>
+        <f>Forecast_Data!AH1</f>
         <v>Month 8</v>
       </c>
       <c r="J1" s="23" t="str">
-        <f>Forecast_Data!AH1</f>
+        <f>Forecast_Data!AI1</f>
         <v>Month 9</v>
       </c>
       <c r="K1" s="23" t="str">
-        <f>Forecast_Data!AI1</f>
+        <f>Forecast_Data!AJ1</f>
         <v>Month 10</v>
       </c>
       <c r="L1" s="23" t="str">
-        <f>Forecast_Data!AJ1</f>
+        <f>Forecast_Data!AK1</f>
         <v>Month 11</v>
       </c>
       <c r="M1" s="23" t="str">
-        <f>Forecast_Data!AK1</f>
+        <f>Forecast_Data!AL1</f>
         <v>Month 12</v>
       </c>
     </row>
@@ -6003,51 +6010,51 @@
         <v>26</v>
       </c>
       <c r="B2" s="17">
-        <f>Forecast_Data!Z8</f>
+        <f>Forecast_Data!AA8</f>
         <v>0</v>
       </c>
       <c r="C2" s="17">
-        <f>Forecast_Data!AA8</f>
+        <f>Forecast_Data!AB8</f>
         <v>0</v>
       </c>
       <c r="D2" s="17">
-        <f>Forecast_Data!AB8</f>
+        <f>Forecast_Data!AC8</f>
         <v>0</v>
       </c>
       <c r="E2" s="17">
-        <f>Forecast_Data!AC8</f>
+        <f>Forecast_Data!AD8</f>
         <v>0</v>
       </c>
       <c r="F2" s="17">
-        <f>Forecast_Data!AD8</f>
+        <f>Forecast_Data!AE8</f>
         <v>0</v>
       </c>
       <c r="G2" s="17">
-        <f>Forecast_Data!AE8</f>
+        <f>Forecast_Data!AF8</f>
         <v>0</v>
       </c>
       <c r="H2" s="17">
-        <f>Forecast_Data!AF8</f>
+        <f>Forecast_Data!AG8</f>
         <v>0</v>
       </c>
       <c r="I2" s="17">
-        <f>Forecast_Data!AG8</f>
+        <f>Forecast_Data!AH8</f>
         <v>0</v>
       </c>
       <c r="J2" s="17">
-        <f>Forecast_Data!AH8</f>
+        <f>Forecast_Data!AI8</f>
         <v>0</v>
       </c>
       <c r="K2" s="17">
-        <f>Forecast_Data!AI8</f>
+        <f>Forecast_Data!AJ8</f>
         <v>0</v>
       </c>
       <c r="L2" s="17">
-        <f>Forecast_Data!AJ8</f>
+        <f>Forecast_Data!AK8</f>
         <v>0</v>
       </c>
       <c r="M2" s="17">
-        <f>Forecast_Data!AK8</f>
+        <f>Forecast_Data!AL8</f>
         <v>0</v>
       </c>
     </row>
@@ -6056,51 +6063,51 @@
         <v>25</v>
       </c>
       <c r="B3" s="18">
-        <f>Forecast_Data!Z7</f>
+        <f>Forecast_Data!AA7</f>
         <v>0</v>
       </c>
       <c r="C3" s="18">
-        <f>Forecast_Data!AA7</f>
+        <f>Forecast_Data!AB7</f>
         <v>0</v>
       </c>
       <c r="D3" s="18">
-        <f>Forecast_Data!AB7</f>
+        <f>Forecast_Data!AC7</f>
         <v>0</v>
       </c>
       <c r="E3" s="18">
-        <f>Forecast_Data!AC7</f>
+        <f>Forecast_Data!AD7</f>
         <v>0</v>
       </c>
       <c r="F3" s="18">
-        <f>Forecast_Data!AD7</f>
+        <f>Forecast_Data!AE7</f>
         <v>0</v>
       </c>
       <c r="G3" s="18">
-        <f>Forecast_Data!AE7</f>
+        <f>Forecast_Data!AF7</f>
         <v>0</v>
       </c>
       <c r="H3" s="18">
-        <f>Forecast_Data!AF7</f>
+        <f>Forecast_Data!AG7</f>
         <v>0</v>
       </c>
       <c r="I3" s="18">
-        <f>Forecast_Data!AG7</f>
+        <f>Forecast_Data!AH7</f>
         <v>0</v>
       </c>
       <c r="J3" s="18">
-        <f>Forecast_Data!AH7</f>
+        <f>Forecast_Data!AI7</f>
         <v>0</v>
       </c>
       <c r="K3" s="18">
-        <f>Forecast_Data!AI7</f>
+        <f>Forecast_Data!AJ7</f>
         <v>0</v>
       </c>
       <c r="L3" s="18">
-        <f>Forecast_Data!AJ7</f>
+        <f>Forecast_Data!AK7</f>
         <v>0</v>
       </c>
       <c r="M3" s="18">
-        <f>Forecast_Data!AK7</f>
+        <f>Forecast_Data!AL7</f>
         <v>0</v>
       </c>
     </row>
@@ -6215,51 +6222,51 @@
         <v>30</v>
       </c>
       <c r="B6" s="19">
-        <f>Forecast_Data!Z9</f>
+        <f>Forecast_Data!AA9</f>
         <v>0</v>
       </c>
       <c r="C6" s="19">
-        <f>B6+Forecast_Data!AA9</f>
+        <f>B6+Forecast_Data!AB9</f>
         <v>0</v>
       </c>
       <c r="D6" s="19">
-        <f>C6+Forecast_Data!AB9</f>
+        <f>C6+Forecast_Data!AC9</f>
         <v>0</v>
       </c>
       <c r="E6" s="19">
-        <f>D6+Forecast_Data!AC9</f>
+        <f>D6+Forecast_Data!AD9</f>
         <v>0</v>
       </c>
       <c r="F6" s="19">
-        <f>E6+Forecast_Data!AD9</f>
+        <f>E6+Forecast_Data!AE9</f>
         <v>0</v>
       </c>
       <c r="G6" s="19">
-        <f>F6+Forecast_Data!AE9</f>
+        <f>F6+Forecast_Data!AF9</f>
         <v>0</v>
       </c>
       <c r="H6" s="19">
-        <f>G6+Forecast_Data!AF9</f>
+        <f>G6+Forecast_Data!AG9</f>
         <v>0</v>
       </c>
       <c r="I6" s="19">
-        <f>H6+Forecast_Data!AG9</f>
+        <f>H6+Forecast_Data!AH9</f>
         <v>0</v>
       </c>
       <c r="J6" s="19">
-        <f>I6+Forecast_Data!AH9</f>
+        <f>I6+Forecast_Data!AI9</f>
         <v>0</v>
       </c>
       <c r="K6" s="19">
-        <f>J6+Forecast_Data!AI9</f>
+        <f>J6+Forecast_Data!AJ9</f>
         <v>0</v>
       </c>
       <c r="L6" s="19">
-        <f>K6+Forecast_Data!AJ9</f>
+        <f>K6+Forecast_Data!AK9</f>
         <v>0</v>
       </c>
       <c r="M6" s="19">
-        <f>L6+Forecast_Data!AK9</f>
+        <f>L6+Forecast_Data!AL9</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ForecastExport/ForecastTemplate: Planning data fixed.
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C130170-7425-0246-B95A-A00FC282BC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410A4F23-C152-8E4F-824F-7EFA337A2682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1631,6 +1631,82 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-B32B-A944-8796-DC91D72BEAD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Vorjahr</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Umsatz kumuliert'!$B$8:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00" €"</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1C79-C54F-97EE-FC7D87589FA6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4912,17 +4988,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> Die IST-Daten im aktuellen</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Monat dienen nur der Information und dürfen nicht dem Monatsprognosewert hinzugefügt werden!</a:t>
+            <a:t> Im aktuellen Monat wird der größere Wert verwendet: Die IST-Daten (Rechnungen) oder der Monatsforecast.</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE" sz="1100">
             <a:solidFill>
@@ -5411,7 +5477,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA9" sqref="AA9"/>
+      <selection pane="bottomRight" activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5842,7 +5908,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.15">
       <c r="Z7" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AA7" s="9">
         <f t="shared" ref="AA7:AL7" si="6">SUM(AA2:AA6)</f>
@@ -6020,7 +6086,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6232,51 +6298,51 @@
         <v>28</v>
       </c>
       <c r="B4" s="18">
-        <f t="shared" ref="B4" si="0">IF(B2 &gt; 0,B2,B3)</f>
+        <f>MAX(B2,B3)</f>
         <v>0</v>
       </c>
       <c r="C4" s="18">
-        <f>IF(C2 &gt; C3,C2,C3)</f>
+        <f t="shared" ref="C4:M4" si="0">MAX(C2,C3)</f>
         <v>0</v>
       </c>
       <c r="D4" s="18">
-        <f t="shared" ref="D4:M4" si="1">IF(D2 &gt; D3,D2,D3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M4" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6293,43 +6359,43 @@
         <v>0</v>
       </c>
       <c r="D5" s="19">
-        <f t="shared" ref="D5:M5" si="2">C5+D4</f>
+        <f t="shared" ref="D5:M5" si="1">C5+D4</f>
         <v>0</v>
       </c>
       <c r="E5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M5" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6465,43 +6531,43 @@
         <v>0</v>
       </c>
       <c r="D9" s="25">
-        <f t="shared" ref="D9:M9" si="3">C9+D8</f>
+        <f t="shared" ref="D9:M9" si="2">C9+D8</f>
         <v>0</v>
       </c>
       <c r="E9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M9" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6717,10 +6783,10 @@
   <dimension ref="A1:AR9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z9" sqref="Z9"/>
+      <selection pane="bottomRight" activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7151,14 +7217,14 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.15">
       <c r="Z7" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AA7" s="16">
-        <f t="shared" ref="AA7:AL7" si="5">SUM(AA2:AA6)</f>
+        <f>MAX(SUM(AA2:AA6),AA8)</f>
         <v>0</v>
       </c>
       <c r="AB7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AB7:AL7" si="5">MAX(SUM(AB2:AB6),AB8)</f>
         <v>0</v>
       </c>
       <c r="AC7" s="16">

</xml_diff>

<commit_message>
Forecast and orderbook: forecast-Type for orders/positions added (current month or following month)
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410A4F23-C152-8E4F-824F-7EFA337A2682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35B887E-C8ED-784C-AA38-7D5D4D08C1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="__xlfn_SUMIFS">#N/A</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AL$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AM$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Planning_Data!$A$1:$AL$9</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -67,7 +67,7 @@
     gewichtete Nettosumme abzügiich bereits faktuierter Beträge</t>
       </text>
     </comment>
-    <comment ref="W1" authorId="2" shapeId="0" xr:uid="{A8EB9EF4-9E59-0C48-894D-F722617BD399}">
+    <comment ref="X1" authorId="2" shapeId="0" xr:uid="{A8EB9EF4-9E59-0C48-894D-F722617BD399}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -75,7 +75,7 @@
     Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="3" shapeId="0" xr:uid="{6BA95036-6D30-5548-82CC-FCCC89EFA3EF}">
+    <comment ref="Y1" authorId="3" shapeId="0" xr:uid="{6BA95036-6D30-5548-82CC-FCCC89EFA3EF}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="92">
   <si>
     <t>Nr.</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Planning date</t>
+  </si>
+  <si>
+    <t>Forecasttyp</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1011,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$2:$AL$2</c:f>
+              <c:f>Forecast_Data!$AB$2:$AM$2</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1097,7 +1100,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$4:$AL$4</c:f>
+              <c:f>Forecast_Data!$AB$4:$AM$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1186,7 +1189,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$3:$AL$3</c:f>
+              <c:f>Forecast_Data!$AB$3:$AM$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1275,7 +1278,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$6:$AL$6</c:f>
+              <c:f>Forecast_Data!$AB$6:$AM$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1366,7 +1369,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$5:$AL$5</c:f>
+              <c:f>Forecast_Data!$AB$5:$AM$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1441,7 +1444,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$8:$AL$8</c:f>
+              <c:f>Forecast_Data!$AB$8:$AM$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1511,7 +1514,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Forecast_Data!$Z$9</c:f>
+              <c:f>Forecast_Data!$AA$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1540,7 +1543,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Forecast_Data!$AA$1:$AL$1</c:f>
+              <c:f>Forecast_Data!$AB$1:$AM$1</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1584,7 +1587,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$9:$AL$9</c:f>
+              <c:f>Forecast_Data!$AB$9:$AM$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2954,7 +2957,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Forecast_Data!$Z$9</c:f>
+              <c:f>Forecast_Data!$AA$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2986,7 +2989,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AA$9:$AL$9</c:f>
+              <c:f>Forecast_Data!$AB$9:$AM$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5443,10 +5446,10 @@
   <threadedComment ref="Q1" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{05417129-CD48-C74E-9020-C754C6816560}">
     <text>gewichtete Nettosumme abzügiich bereits faktuierter Beträge</text>
   </threadedComment>
-  <threadedComment ref="W1" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{A8EB9EF4-9E59-0C48-894D-F722617BD399}">
+  <threadedComment ref="X1" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{A8EB9EF4-9E59-0C48-894D-F722617BD399}">
     <text>Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</text>
   </threadedComment>
-  <threadedComment ref="X1" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{6BA95036-6D30-5548-82CC-FCCC89EFA3EF}">
+  <threadedComment ref="Y1" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{6BA95036-6D30-5548-82CC-FCCC89EFA3EF}">
     <text>Das Budget ist um den angegebenen Betrag unter- (negative Werte) oder überschritten (positive Werte)</text>
   </threadedComment>
 </ThreadedComments>
@@ -5471,13 +5474,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR9"/>
+  <dimension ref="A1:AS9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA10" sqref="AA10"/>
+      <selection pane="bottomRight" activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5496,20 +5499,20 @@
     <col min="16" max="18" width="11.5" style="2" customWidth="1"/>
     <col min="19" max="19" width="11.5" style="20" customWidth="1"/>
     <col min="20" max="21" width="11.5" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" style="25" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" style="25" customWidth="1"/>
-    <col min="25" max="25" width="11.5" customWidth="1"/>
-    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="38" width="12.83203125" style="2" customWidth="1"/>
-    <col min="39" max="40" width="19" style="1" customWidth="1"/>
-    <col min="41" max="41" width="52.83203125" customWidth="1"/>
-    <col min="42" max="42" width="16.5" customWidth="1"/>
-    <col min="43" max="43" width="29.5" customWidth="1"/>
-    <col min="44" max="44" width="65.6640625" customWidth="1"/>
+    <col min="22" max="23" width="8" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" style="25" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.5" customWidth="1"/>
+    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="39" width="12.83203125" style="2" customWidth="1"/>
+    <col min="40" max="41" width="19" style="1" customWidth="1"/>
+    <col min="42" max="42" width="52.83203125" customWidth="1"/>
+    <col min="43" max="43" width="16.5" customWidth="1"/>
+    <col min="44" max="44" width="29.5" customWidth="1"/>
+    <col min="45" max="45" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:45" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5574,83 +5577,82 @@
       <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="22" t="s">
+      <c r="AN1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AN1" s="22" t="s">
+      <c r="AO1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="26" t="s">
+      <c r="AP1" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:45" ht="20" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="7">
-        <f t="shared" ref="AA2:AL2" si="0">SUMIFS(AA10:AA65537,$K10:$K65537,"=beauftragt")</f>
-        <v>0</v>
-      </c>
       <c r="AB2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AB2:AM2" si="0">SUMIFS(AB10:AB65537,$K10:$K65537,"=beauftragt")</f>
         <v>0</v>
       </c>
       <c r="AC2" s="7">
@@ -5693,17 +5695,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AM2" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z3" s="8" t="s">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AA3" s="9">
-        <f t="shared" ref="AA3:AL3" si="1">SUMIFS(AA10:AA65537,$K10:$K65537,"=gelegt")</f>
-        <v>0</v>
-      </c>
       <c r="AB3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AB3:AM3" si="1">SUMIFS(AB10:AB65537,$K10:$K65537,"=gelegt")</f>
         <v>0</v>
       </c>
       <c r="AC3" s="9">
@@ -5746,17 +5748,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AM3" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z4" s="6" t="s">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AA4" s="7">
-        <f t="shared" ref="AA4:AL4" si="2">SUMIFS(AA10:AA65537,$K10:$K65537,"=LOI")</f>
-        <v>0</v>
-      </c>
       <c r="AB4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AB4:AM4" si="2">SUMIFS(AB10:AB65537,$K10:$K65537,"=LOI")</f>
         <v>0</v>
       </c>
       <c r="AC4" s="7">
@@ -5799,17 +5801,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AM4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z5" s="8" t="s">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AA5" s="9">
-        <f t="shared" ref="AA5:AF5" si="3">SUMIFS(AA10:AA65537,$K10:$K65537,"=in Erstellung")</f>
-        <v>0</v>
-      </c>
       <c r="AB5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AB5:AG5" si="3">SUMIFS(AB10:AB65537,$K10:$K65537,"=in Erstellung")</f>
         <v>0</v>
       </c>
       <c r="AC5" s="9">
@@ -5829,11 +5831,11 @@
         <v>0</v>
       </c>
       <c r="AG5" s="9">
-        <f t="shared" ref="AG5:AL5" si="4">SUMIFS(AG10:AG65537,$K10:$K65537,"=in Erstellung")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH5" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AH5:AM5" si="4">SUMIFS(AH10:AH65537,$K10:$K65537,"=in Erstellung")</f>
         <v>0</v>
       </c>
       <c r="AI5" s="9">
@@ -5852,17 +5854,17 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="AM5" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z6" s="10" t="s">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AA6" s="11">
-        <f t="shared" ref="AA6:AL6" si="5">SUMIFS(AA10:AA65537,$K10:$K65537,"=Potenzial")</f>
-        <v>0</v>
-      </c>
       <c r="AB6" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AB6:AM6" si="5">SUMIFS(AB10:AB65537,$K10:$K65537,"=Potenzial")</f>
         <v>0</v>
       </c>
       <c r="AC6" s="11">
@@ -5905,17 +5907,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="AM6" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z7" s="12" t="s">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AA7" s="9">
-        <f t="shared" ref="AA7:AL7" si="6">SUM(AA2:AA6)</f>
-        <v>0</v>
-      </c>
       <c r="AB7" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AB7:AM7" si="6">SUM(AB2:AB6)</f>
         <v>0</v>
       </c>
       <c r="AC7" s="9">
@@ -5958,109 +5960,113 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AM7" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z8" s="13" t="s">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AA8" s="14">
+      <c r="AB8" s="14">
         <f>SUM(Rechnungen!M2:M65535)</f>
         <v>0</v>
       </c>
-      <c r="AB8" s="14">
+      <c r="AC8" s="14">
         <f>SUM(Rechnungen!N2:N65535)</f>
         <v>0</v>
       </c>
-      <c r="AC8" s="14">
+      <c r="AD8" s="14">
         <f>SUM(Rechnungen!O2:O65535)</f>
         <v>0</v>
       </c>
-      <c r="AD8" s="14">
+      <c r="AE8" s="14">
         <f>SUM(Rechnungen!P2:P65535)</f>
         <v>0</v>
       </c>
-      <c r="AE8" s="14">
+      <c r="AF8" s="14">
         <f>SUM(Rechnungen!Q2:Q65535)</f>
         <v>0</v>
       </c>
-      <c r="AF8" s="14">
+      <c r="AG8" s="14">
         <f>SUM(Rechnungen!R2:R65535)</f>
         <v>0</v>
       </c>
-      <c r="AG8" s="14">
+      <c r="AH8" s="14">
         <f>SUM(Rechnungen!S2:S65535)</f>
         <v>0</v>
       </c>
-      <c r="AH8" s="14">
+      <c r="AI8" s="14">
         <f>SUM(Rechnungen!T2:T65535)</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="14">
+      <c r="AJ8" s="14">
         <f>SUM(Rechnungen!U2:U65535)</f>
         <v>0</v>
       </c>
-      <c r="AJ8" s="14">
+      <c r="AK8" s="14">
         <f>SUM(Rechnungen!V2:V65535)</f>
         <v>0</v>
       </c>
-      <c r="AK8" s="14">
+      <c r="AL8" s="14">
         <f>SUM(Rechnungen!W2:W65535)</f>
         <v>0</v>
       </c>
-      <c r="AL8" s="14">
+      <c r="AM8" s="14">
         <f>SUM(Rechnungen!X2:X65535)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z9" s="15" t="s">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AA9" s="16">
+      <c r="AB9" s="16">
         <f>Planning_Data!AA7</f>
         <v>0</v>
       </c>
-      <c r="AB9" s="16">
+      <c r="AC9" s="16">
         <f>Planning_Data!AB7</f>
         <v>0</v>
       </c>
-      <c r="AC9" s="16">
+      <c r="AD9" s="16">
         <f>Planning_Data!AC7</f>
         <v>0</v>
       </c>
-      <c r="AD9" s="16">
+      <c r="AE9" s="16">
         <f>Planning_Data!AD7</f>
         <v>0</v>
       </c>
-      <c r="AE9" s="16">
+      <c r="AF9" s="16">
         <f>Planning_Data!AE7</f>
         <v>0</v>
       </c>
-      <c r="AF9" s="16">
+      <c r="AG9" s="16">
         <f>Planning_Data!AF7</f>
         <v>0</v>
       </c>
-      <c r="AG9" s="16">
+      <c r="AH9" s="16">
         <f>Planning_Data!AG7</f>
         <v>0</v>
       </c>
-      <c r="AH9" s="16">
+      <c r="AI9" s="16">
         <f>Planning_Data!AH7</f>
         <v>0</v>
       </c>
-      <c r="AI9" s="16">
+      <c r="AJ9" s="16">
         <f>Planning_Data!AI7</f>
         <v>0</v>
       </c>
-      <c r="AJ9" s="16">
+      <c r="AK9" s="16">
         <f>Planning_Data!AJ7</f>
         <v>0</v>
       </c>
-      <c r="AK9" s="16">
+      <c r="AL9" s="16">
         <f>Planning_Data!AK7</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="16">
+      <c r="AM9" s="16">
         <f>Planning_Data!AL7</f>
         <v>0</v>
       </c>
@@ -6139,51 +6145,51 @@
   <sheetData>
     <row r="1" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B1" s="23" t="str">
-        <f>Forecast_Data!AA1</f>
+        <f>Forecast_Data!AB1</f>
         <v>Month 1</v>
       </c>
       <c r="C1" s="23" t="str">
-        <f>Forecast_Data!AB1</f>
+        <f>Forecast_Data!AC1</f>
         <v>Month 2</v>
       </c>
       <c r="D1" s="23" t="str">
-        <f>Forecast_Data!AC1</f>
+        <f>Forecast_Data!AD1</f>
         <v>Month 3</v>
       </c>
       <c r="E1" s="23" t="str">
-        <f>Forecast_Data!AD1</f>
+        <f>Forecast_Data!AE1</f>
         <v>Month 4</v>
       </c>
       <c r="F1" s="23" t="str">
-        <f>Forecast_Data!AE1</f>
+        <f>Forecast_Data!AF1</f>
         <v>Month 5</v>
       </c>
       <c r="G1" s="23" t="str">
-        <f>Forecast_Data!AF1</f>
+        <f>Forecast_Data!AG1</f>
         <v>Month 6</v>
       </c>
       <c r="H1" s="23" t="str">
-        <f>Forecast_Data!AG1</f>
+        <f>Forecast_Data!AH1</f>
         <v>Month 7</v>
       </c>
       <c r="I1" s="23" t="str">
-        <f>Forecast_Data!AH1</f>
+        <f>Forecast_Data!AI1</f>
         <v>Month 8</v>
       </c>
       <c r="J1" s="23" t="str">
-        <f>Forecast_Data!AI1</f>
+        <f>Forecast_Data!AJ1</f>
         <v>Month 9</v>
       </c>
       <c r="K1" s="23" t="str">
-        <f>Forecast_Data!AJ1</f>
+        <f>Forecast_Data!AK1</f>
         <v>Month 10</v>
       </c>
       <c r="L1" s="23" t="str">
-        <f>Forecast_Data!AK1</f>
+        <f>Forecast_Data!AL1</f>
         <v>Month 11</v>
       </c>
       <c r="M1" s="23" t="str">
-        <f>Forecast_Data!AL1</f>
+        <f>Forecast_Data!AM1</f>
         <v>Month 12</v>
       </c>
     </row>
@@ -6192,51 +6198,51 @@
         <v>26</v>
       </c>
       <c r="B2" s="17">
-        <f>Forecast_Data!AA8</f>
+        <f>Forecast_Data!AB8</f>
         <v>0</v>
       </c>
       <c r="C2" s="17">
-        <f>Forecast_Data!AB8</f>
+        <f>Forecast_Data!AC8</f>
         <v>0</v>
       </c>
       <c r="D2" s="17">
-        <f>Forecast_Data!AC8</f>
+        <f>Forecast_Data!AD8</f>
         <v>0</v>
       </c>
       <c r="E2" s="17">
-        <f>Forecast_Data!AD8</f>
+        <f>Forecast_Data!AE8</f>
         <v>0</v>
       </c>
       <c r="F2" s="17">
-        <f>Forecast_Data!AE8</f>
+        <f>Forecast_Data!AF8</f>
         <v>0</v>
       </c>
       <c r="G2" s="17">
-        <f>Forecast_Data!AF8</f>
+        <f>Forecast_Data!AG8</f>
         <v>0</v>
       </c>
       <c r="H2" s="17">
-        <f>Forecast_Data!AG8</f>
+        <f>Forecast_Data!AH8</f>
         <v>0</v>
       </c>
       <c r="I2" s="17">
-        <f>Forecast_Data!AH8</f>
+        <f>Forecast_Data!AI8</f>
         <v>0</v>
       </c>
       <c r="J2" s="17">
-        <f>Forecast_Data!AI8</f>
+        <f>Forecast_Data!AJ8</f>
         <v>0</v>
       </c>
       <c r="K2" s="17">
-        <f>Forecast_Data!AJ8</f>
+        <f>Forecast_Data!AK8</f>
         <v>0</v>
       </c>
       <c r="L2" s="17">
-        <f>Forecast_Data!AK8</f>
+        <f>Forecast_Data!AL8</f>
         <v>0</v>
       </c>
       <c r="M2" s="17">
-        <f>Forecast_Data!AL8</f>
+        <f>Forecast_Data!AM8</f>
         <v>0</v>
       </c>
     </row>
@@ -6245,51 +6251,51 @@
         <v>25</v>
       </c>
       <c r="B3" s="18">
-        <f>Forecast_Data!AA7</f>
+        <f>Forecast_Data!AB7</f>
         <v>0</v>
       </c>
       <c r="C3" s="18">
-        <f>Forecast_Data!AB7</f>
+        <f>Forecast_Data!AC7</f>
         <v>0</v>
       </c>
       <c r="D3" s="18">
-        <f>Forecast_Data!AC7</f>
+        <f>Forecast_Data!AD7</f>
         <v>0</v>
       </c>
       <c r="E3" s="18">
-        <f>Forecast_Data!AD7</f>
+        <f>Forecast_Data!AE7</f>
         <v>0</v>
       </c>
       <c r="F3" s="18">
-        <f>Forecast_Data!AE7</f>
+        <f>Forecast_Data!AF7</f>
         <v>0</v>
       </c>
       <c r="G3" s="18">
-        <f>Forecast_Data!AF7</f>
+        <f>Forecast_Data!AG7</f>
         <v>0</v>
       </c>
       <c r="H3" s="18">
-        <f>Forecast_Data!AG7</f>
+        <f>Forecast_Data!AH7</f>
         <v>0</v>
       </c>
       <c r="I3" s="18">
-        <f>Forecast_Data!AH7</f>
+        <f>Forecast_Data!AI7</f>
         <v>0</v>
       </c>
       <c r="J3" s="18">
-        <f>Forecast_Data!AI7</f>
+        <f>Forecast_Data!AJ7</f>
         <v>0</v>
       </c>
       <c r="K3" s="18">
-        <f>Forecast_Data!AJ7</f>
+        <f>Forecast_Data!AK7</f>
         <v>0</v>
       </c>
       <c r="L3" s="18">
-        <f>Forecast_Data!AK7</f>
+        <f>Forecast_Data!AL7</f>
         <v>0</v>
       </c>
       <c r="M3" s="18">
-        <f>Forecast_Data!AL7</f>
+        <f>Forecast_Data!AM7</f>
         <v>0</v>
       </c>
     </row>
@@ -6404,51 +6410,51 @@
         <v>30</v>
       </c>
       <c r="B6" s="19">
-        <f>Forecast_Data!AA9</f>
+        <f>Forecast_Data!AB9</f>
         <v>0</v>
       </c>
       <c r="C6" s="19">
-        <f>B6+Forecast_Data!AB9</f>
+        <f>B6+Forecast_Data!AC9</f>
         <v>0</v>
       </c>
       <c r="D6" s="19">
-        <f>C6+Forecast_Data!AC9</f>
+        <f>C6+Forecast_Data!AD9</f>
         <v>0</v>
       </c>
       <c r="E6" s="19">
-        <f>D6+Forecast_Data!AD9</f>
+        <f>D6+Forecast_Data!AE9</f>
         <v>0</v>
       </c>
       <c r="F6" s="19">
-        <f>E6+Forecast_Data!AE9</f>
+        <f>E6+Forecast_Data!AF9</f>
         <v>0</v>
       </c>
       <c r="G6" s="19">
-        <f>F6+Forecast_Data!AF9</f>
+        <f>F6+Forecast_Data!AG9</f>
         <v>0</v>
       </c>
       <c r="H6" s="19">
-        <f>G6+Forecast_Data!AG9</f>
+        <f>G6+Forecast_Data!AH9</f>
         <v>0</v>
       </c>
       <c r="I6" s="19">
-        <f>H6+Forecast_Data!AH9</f>
+        <f>H6+Forecast_Data!AI9</f>
         <v>0</v>
       </c>
       <c r="J6" s="19">
-        <f>I6+Forecast_Data!AI9</f>
+        <f>I6+Forecast_Data!AJ9</f>
         <v>0</v>
       </c>
       <c r="K6" s="19">
-        <f>J6+Forecast_Data!AJ9</f>
+        <f>J6+Forecast_Data!AK9</f>
         <v>0</v>
       </c>
       <c r="L6" s="19">
-        <f>K6+Forecast_Data!AK9</f>
+        <f>K6+Forecast_Data!AL9</f>
         <v>0</v>
       </c>
       <c r="M6" s="19">
-        <f>L6+Forecast_Data!AL9</f>
+        <f>L6+Forecast_Data!AM9</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Forecast improved, html package extended.
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35B887E-C8ED-784C-AA38-7D5D4D08C1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9A5F97-5F6C-394D-8C27-313E6F5232B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="__xlfn_SUMIFS">#N/A</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AM$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Planning_Data!$A$1:$AL$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Planning_Data!$A$1:$AM$9</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -112,7 +112,7 @@
     gewichtete Nettosumme abzügiich bereits faktuierter Beträge</t>
       </text>
     </comment>
-    <comment ref="W1" authorId="2" shapeId="0" xr:uid="{6F893BEE-C504-044C-9481-4570AAFDCB74}">
+    <comment ref="X1" authorId="2" shapeId="0" xr:uid="{6F893BEE-C504-044C-9481-4570AAFDCB74}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -120,7 +120,7 @@
     Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="3" shapeId="0" xr:uid="{5DE2B462-19A1-4A4E-9F4A-C3A45444414B}">
+    <comment ref="Y1" authorId="3" shapeId="0" xr:uid="{5DE2B462-19A1-4A4E-9F4A-C3A45444414B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -133,12 +133,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="95">
   <si>
     <t>Nr.</t>
-  </si>
-  <si>
-    <t>Angebotsdatum</t>
   </si>
   <si>
     <t>Erfassungsdatum</t>
@@ -411,6 +408,90 @@
   </si>
   <si>
     <t>Forecasttyp</t>
+  </si>
+  <si>
+    <t>Angebotsdatum</t>
+  </si>
+  <si>
+    <t>Probality / Wahrscheinlichkeit</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>payment plan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is used first, if available.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Fixed price projects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> are scheduled at the end of the performance period.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Time and materials</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Flat-rate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> projects are distributed monthly during the performance period.</t>
+    </r>
+  </si>
+  <si>
+    <t>Distribution of Forecast / Monatsverteilung</t>
   </si>
 </sst>
 </file>
@@ -712,7 +793,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -772,13 +853,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -5463,10 +5550,10 @@
   <threadedComment ref="Q1" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{9099E2DF-84A2-AB44-BB64-42C60828BEA6}">
     <text>gewichtete Nettosumme abzügiich bereits faktuierter Beträge</text>
   </threadedComment>
-  <threadedComment ref="W1" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{6F893BEE-C504-044C-9481-4570AAFDCB74}">
+  <threadedComment ref="X1" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{6F893BEE-C504-044C-9481-4570AAFDCB74}">
     <text>Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</text>
   </threadedComment>
-  <threadedComment ref="X1" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{5DE2B462-19A1-4A4E-9F4A-C3A45444414B}">
+  <threadedComment ref="Y1" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{5DE2B462-19A1-4A4E-9F4A-C3A45444414B}">
     <text>Das Budget ist um den angegebenen Betrag unter- (negative Werte) oder überschritten (positive Werte)</text>
   </threadedComment>
 </ThreadedComments>
@@ -5477,8 +5564,8 @@
   <dimension ref="A1:AS9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AB9" sqref="AB9"/>
     </sheetView>
@@ -5487,9 +5574,9 @@
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
     <col min="6" max="7" width="31.1640625" customWidth="1"/>
     <col min="8" max="11" width="11.5" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" customWidth="1"/>
@@ -5517,139 +5604,141 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="33" t="s">
         <v>14</v>
-      </c>
-      <c r="T1" s="33" t="s">
-        <v>15</v>
       </c>
       <c r="U1" s="33"/>
       <c r="V1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X1" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y1" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="Y1" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="AA1" s="3"/>
       <c r="AB1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="AH1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="AN1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AO1" s="22" t="s">
-        <v>3</v>
-      </c>
       <c r="AP1" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AQ1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>18</v>
-      </c>
-      <c r="AS1" s="21" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:45" ht="20" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
+      <c r="A2" s="34">
+        <v>45658</v>
+      </c>
       <c r="B2" s="34"/>
       <c r="AA2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AB2" s="7">
         <f t="shared" ref="AB2:AM2" si="0">SUMIFS(AB10:AB65537,$K10:$K65537,"=beauftragt")</f>
@@ -5702,7 +5791,7 @@
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AB3" s="9">
         <f t="shared" ref="AB3:AM3" si="1">SUMIFS(AB10:AB65537,$K10:$K65537,"=gelegt")</f>
@@ -5755,7 +5844,7 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" ref="AB4:AM4" si="2">SUMIFS(AB10:AB65537,$K10:$K65537,"=LOI")</f>
@@ -5808,7 +5897,7 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB5" s="9">
         <f t="shared" ref="AB5:AG5" si="3">SUMIFS(AB10:AB65537,$K10:$K65537,"=in Erstellung")</f>
@@ -5861,7 +5950,7 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA6" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AB6" s="11">
         <f t="shared" ref="AB6:AM6" si="5">SUMIFS(AB10:AB65537,$K10:$K65537,"=Potenzial")</f>
@@ -5914,7 +6003,7 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA7" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB7" s="9">
         <f t="shared" ref="AB7:AM7" si="6">SUM(AB2:AB6)</f>
@@ -5967,7 +6056,7 @@
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA8" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AB8" s="14">
         <f>SUM(Rechnungen!M2:M65535)</f>
@@ -6020,54 +6109,54 @@
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA9" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB9" s="16">
-        <f>Planning_Data!AA7</f>
+        <f>Planning_Data!AB7</f>
         <v>0</v>
       </c>
       <c r="AC9" s="16">
-        <f>Planning_Data!AB7</f>
+        <f>Planning_Data!AC7</f>
         <v>0</v>
       </c>
       <c r="AD9" s="16">
-        <f>Planning_Data!AC7</f>
+        <f>Planning_Data!AD7</f>
         <v>0</v>
       </c>
       <c r="AE9" s="16">
-        <f>Planning_Data!AD7</f>
+        <f>Planning_Data!AE7</f>
         <v>0</v>
       </c>
       <c r="AF9" s="16">
-        <f>Planning_Data!AE7</f>
+        <f>Planning_Data!AF7</f>
         <v>0</v>
       </c>
       <c r="AG9" s="16">
-        <f>Planning_Data!AF7</f>
+        <f>Planning_Data!AG7</f>
         <v>0</v>
       </c>
       <c r="AH9" s="16">
-        <f>Planning_Data!AG7</f>
+        <f>Planning_Data!AH7</f>
         <v>0</v>
       </c>
       <c r="AI9" s="16">
-        <f>Planning_Data!AH7</f>
+        <f>Planning_Data!AI7</f>
         <v>0</v>
       </c>
       <c r="AJ9" s="16">
-        <f>Planning_Data!AI7</f>
+        <f>Planning_Data!AJ7</f>
         <v>0</v>
       </c>
       <c r="AK9" s="16">
-        <f>Planning_Data!AJ7</f>
+        <f>Planning_Data!AK7</f>
         <v>0</v>
       </c>
       <c r="AL9" s="16">
-        <f>Planning_Data!AK7</f>
+        <f>Planning_Data!AL7</f>
         <v>0</v>
       </c>
       <c r="AM9" s="16">
-        <f>Planning_Data!AL7</f>
+        <f>Planning_Data!AM7</f>
         <v>0</v>
       </c>
     </row>
@@ -6195,7 +6284,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="17">
         <f>Forecast_Data!AB8</f>
@@ -6248,7 +6337,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="18">
         <f>Forecast_Data!AB7</f>
@@ -6301,7 +6390,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="18">
         <f>MAX(B2,B3)</f>
@@ -6354,7 +6443,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="19">
         <f>B4</f>
@@ -6407,7 +6496,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="19">
         <f>Forecast_Data!AB9</f>
@@ -6473,7 +6562,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="19">
         <f>SUM('Rechnungen Vorjahr'!M2:M65534)</f>
@@ -6526,7 +6615,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="19">
         <f>B8</f>
@@ -6609,71 +6698,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="I1" s="35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="S1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -6709,71 +6798,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="I1" s="35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="S1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -6786,22 +6875,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AD000D-C6FB-164B-AFB3-9CB348DD95B6}">
-  <dimension ref="A1:AR9"/>
+  <dimension ref="A1:AS9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA9" sqref="AA9"/>
+      <selection pane="bottomRight" activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
     <col min="6" max="7" width="31.1640625" customWidth="1"/>
     <col min="8" max="11" width="11.5" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" customWidth="1"/>
@@ -6812,160 +6901,162 @@
     <col min="19" max="19" width="11.5" style="20" customWidth="1"/>
     <col min="20" max="21" width="11.5" style="1" customWidth="1"/>
     <col min="22" max="22" width="8" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" style="25" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" style="25" customWidth="1"/>
-    <col min="25" max="25" width="11.5" customWidth="1"/>
-    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="38" width="12.83203125" style="2" customWidth="1"/>
-    <col min="39" max="40" width="19" style="1" customWidth="1"/>
-    <col min="41" max="41" width="52.83203125" customWidth="1"/>
-    <col min="42" max="42" width="16.5" customWidth="1"/>
-    <col min="43" max="43" width="29.5" customWidth="1"/>
-    <col min="44" max="44" width="65.6640625" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" style="25" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.5" customWidth="1"/>
+    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="39" width="12.83203125" style="2" customWidth="1"/>
+    <col min="40" max="41" width="19" style="1" customWidth="1"/>
+    <col min="42" max="42" width="52.83203125" customWidth="1"/>
+    <col min="43" max="43" width="16.5" customWidth="1"/>
+    <col min="44" max="44" width="29.5" customWidth="1"/>
+    <col min="45" max="45" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:45" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="33" t="s">
         <v>14</v>
-      </c>
-      <c r="T1" s="33" t="s">
-        <v>15</v>
       </c>
       <c r="U1" s="33"/>
       <c r="V1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>88</v>
+        <v>19</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="X1" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="5" t="s">
+      <c r="Y1" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="22" t="s">
+      <c r="AN1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AN1" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO1" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AP1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="21" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:44" ht="20" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
+    <row r="2" spans="1:45" ht="20" x14ac:dyDescent="0.15">
+      <c r="A2" s="34">
+        <v>45658</v>
+      </c>
       <c r="B2" s="34"/>
-      <c r="Z2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA2" s="7">
-        <f t="shared" ref="AA2:AL2" si="0">SUMIFS(AA10:AA65537,$K10:$K65537,"=beauftragt")</f>
-        <v>0</v>
+      <c r="AA2" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="AB2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AB2:AM2" si="0">SUMIFS(AB10:AB65537,$K10:$K65537,"=beauftragt")</f>
         <v>0</v>
       </c>
       <c r="AC2" s="7">
@@ -7008,17 +7099,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AM2" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA3" s="9">
-        <f t="shared" ref="AA3:AL3" si="1">SUMIFS(AA10:AA65537,$K10:$K65537,"=gelegt")</f>
-        <v>0</v>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA3" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="AB3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AB3:AM3" si="1">SUMIFS(AB10:AB65537,$K10:$K65537,"=gelegt")</f>
         <v>0</v>
       </c>
       <c r="AC3" s="9">
@@ -7061,17 +7152,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AM3" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA4" s="7">
-        <f t="shared" ref="AA4:AL4" si="2">SUMIFS(AA10:AA65537,$K10:$K65537,"=LOI")</f>
-        <v>0</v>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA4" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="AB4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AB4:AM4" si="2">SUMIFS(AB10:AB65537,$K10:$K65537,"=LOI")</f>
         <v>0</v>
       </c>
       <c r="AC4" s="7">
@@ -7114,17 +7205,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AM4" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA5" s="9">
-        <f t="shared" ref="AA5:AL5" si="3">SUMIFS(AA10:AA65537,$K10:$K65537,"=in Erstellung")</f>
-        <v>0</v>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA5" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="AB5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AB5:AM5" si="3">SUMIFS(AB10:AB65537,$K10:$K65537,"=in Erstellung")</f>
         <v>0</v>
       </c>
       <c r="AC5" s="9">
@@ -7167,17 +7258,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="AM5" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA6" s="11">
-        <f t="shared" ref="AA6:AL6" si="4">SUMIFS(AA10:AA65537,$K10:$K65537,"=Potenzial")</f>
-        <v>0</v>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA6" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="AB6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AB6:AM6" si="4">SUMIFS(AB10:AB65537,$K10:$K65537,"=Potenzial")</f>
         <v>0</v>
       </c>
       <c r="AC6" s="11">
@@ -7220,21 +7311,21 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="AM6" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z7" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA7" s="16">
-        <f>MAX(SUM(AA2:AA6),AA8)</f>
-        <v>0</v>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA7" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="AB7" s="16">
-        <f t="shared" ref="AB7:AL7" si="5">MAX(SUM(AB2:AB6),AB8)</f>
+        <f>MAX(SUM(AB2:AB6),AB8)</f>
         <v>0</v>
       </c>
       <c r="AC7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AC7:AM7" si="5">MAX(SUM(AC2:AC6),AC8)</f>
         <v>0</v>
       </c>
       <c r="AD7" s="16">
@@ -7273,62 +7364,66 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="AM7" s="16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA8" s="14">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="14">
         <f>SUM(Planning_Invoices!M2:M65535)</f>
         <v>0</v>
       </c>
-      <c r="AB8" s="14">
+      <c r="AC8" s="14">
         <f>SUM(Planning_Invoices!N2:N65535)</f>
         <v>0</v>
       </c>
-      <c r="AC8" s="14">
+      <c r="AD8" s="14">
         <f>SUM(Planning_Invoices!O2:O65535)</f>
         <v>0</v>
       </c>
-      <c r="AD8" s="14">
+      <c r="AE8" s="14">
         <f>SUM(Planning_Invoices!P2:P65535)</f>
         <v>0</v>
       </c>
-      <c r="AE8" s="14">
+      <c r="AF8" s="14">
         <f>SUM(Planning_Invoices!Q2:Q65535)</f>
         <v>0</v>
       </c>
-      <c r="AF8" s="14">
+      <c r="AG8" s="14">
         <f>SUM(Planning_Invoices!R2:R65535)</f>
         <v>0</v>
       </c>
-      <c r="AG8" s="14">
+      <c r="AH8" s="14">
         <f>SUM(Planning_Invoices!S2:S65535)</f>
         <v>0</v>
       </c>
-      <c r="AH8" s="14">
+      <c r="AI8" s="14">
         <f>SUM(Planning_Invoices!T2:T65535)</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="14">
+      <c r="AJ8" s="14">
         <f>SUM(Planning_Invoices!U2:U65535)</f>
         <v>0</v>
       </c>
-      <c r="AJ8" s="14">
+      <c r="AK8" s="14">
         <f>SUM(Planning_Invoices!V2:V65535)</f>
         <v>0</v>
       </c>
-      <c r="AK8" s="14">
+      <c r="AL8" s="14">
         <f>SUM(Planning_Invoices!W2:W65535)</f>
         <v>0</v>
       </c>
-      <c r="AL8" s="14">
+      <c r="AM8" s="14">
         <f>SUM(Planning_Invoices!X2:X65535)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="Z9" s="29"/>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.15">
+      <c r="AA9" s="29"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -7367,71 +7462,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="I1" s="35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="S1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -7445,7 +7540,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB315FBD-69C9-F248-8D6C-0E7BAAF44D90}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -7460,95 +7555,77 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:5" ht="23" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="31"/>
+    </row>
+    <row r="5" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
     </row>
     <row r="6" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="36" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+    </row>
+    <row r="9" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
+      <c r="D11" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -7556,92 +7633,89 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D13">
         <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="D14">
         <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
         <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -7649,137 +7723,140 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="D20">
-        <v>0.9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D21">
-        <v>0.9</v>
-      </c>
-      <c r="E21" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>77</v>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>0.9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24">
+        <v>0.9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -7787,92 +7864,89 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D29">
         <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D30">
         <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -7880,75 +7954,123 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D35">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="D36">
-        <v>0.9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>78</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D37">
-        <v>0.9</v>
-      </c>
-      <c r="E37" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38">
+        <v>0.5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <v>0.9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <v>0.9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41">
         <v>14</v>
       </c>
-      <c r="B38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>78</v>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Forecast Excel export improved.
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9A5F97-5F6C-394D-8C27-313E6F5232B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF07850-C393-8E40-A044-0EBBDD23B5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,13 +45,13 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={ED0F4801-55AC-584A-97BE-17C93D6D0E1F}</author>
-    <author>tc={05417129-CD48-C74E-9020-C754C6816560}</author>
-    <author>tc={A8EB9EF4-9E59-0C48-894D-F722617BD399}</author>
-    <author>tc={6BA95036-6D30-5548-82CC-FCCC89EFA3EF}</author>
+    <author>tc={E45442EF-B789-F747-94A0-67C234C866AE}</author>
+    <author>tc={0E5EDB66-204F-AF48-AF0C-800703AD109B}</author>
+    <author>tc={E18BEFC3-4A25-4C4E-8456-D4AA5435172B}</author>
+    <author>tc={876D63B5-EF23-C74F-AFE0-495EE5563AFA}</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{ED0F4801-55AC-584A-97BE-17C93D6D0E1F}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{E45442EF-B789-F747-94A0-67C234C866AE}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -59,7 +59,7 @@
     Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</t>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{05417129-CD48-C74E-9020-C754C6816560}">
+    <comment ref="Q10" authorId="1" shapeId="0" xr:uid="{0E5EDB66-204F-AF48-AF0C-800703AD109B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -67,7 +67,7 @@
     gewichtete Nettosumme abzügiich bereits faktuierter Beträge</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="2" shapeId="0" xr:uid="{A8EB9EF4-9E59-0C48-894D-F722617BD399}">
+    <comment ref="X10" authorId="2" shapeId="0" xr:uid="{E18BEFC3-4A25-4C4E-8456-D4AA5435172B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -75,7 +75,7 @@
     Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</t>
       </text>
     </comment>
-    <comment ref="Y1" authorId="3" shapeId="0" xr:uid="{6BA95036-6D30-5548-82CC-FCCC89EFA3EF}">
+    <comment ref="Y10" authorId="3" shapeId="0" xr:uid="{876D63B5-EF23-C74F-AFE0-495EE5563AFA}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -90,13 +90,13 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={645A51E0-CF7B-4042-B0FE-74F0618602F1}</author>
-    <author>tc={9099E2DF-84A2-AB44-BB64-42C60828BEA6}</author>
-    <author>tc={6F893BEE-C504-044C-9481-4570AAFDCB74}</author>
-    <author>tc={5DE2B462-19A1-4A4E-9F4A-C3A45444414B}</author>
+    <author>tc={164688EE-C018-C74D-9C06-663D4DFF9926}</author>
+    <author>tc={8A1ADE95-CAA9-B447-9E86-6A4505BBEEA3}</author>
+    <author>tc={DDB2B422-1A98-B042-B162-FC9B5B1C5A39}</author>
+    <author>tc={4BF7C68F-136F-1D47-BEF5-17303DC0469A}</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{645A51E0-CF7B-4042-B0FE-74F0618602F1}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{164688EE-C018-C74D-9C06-663D4DFF9926}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -104,7 +104,7 @@
     Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</t>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{9099E2DF-84A2-AB44-BB64-42C60828BEA6}">
+    <comment ref="Q10" authorId="1" shapeId="0" xr:uid="{8A1ADE95-CAA9-B447-9E86-6A4505BBEEA3}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -112,7 +112,7 @@
     gewichtete Nettosumme abzügiich bereits faktuierter Beträge</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="2" shapeId="0" xr:uid="{6F893BEE-C504-044C-9481-4570AAFDCB74}">
+    <comment ref="X10" authorId="2" shapeId="0" xr:uid="{DDB2B422-1A98-B042-B162-FC9B5B1C5A39}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -120,7 +120,7 @@
     Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</t>
       </text>
     </comment>
-    <comment ref="Y1" authorId="3" shapeId="0" xr:uid="{5DE2B462-19A1-4A4E-9F4A-C3A45444414B}">
+    <comment ref="Y10" authorId="3" shapeId="0" xr:uid="{4BF7C68F-136F-1D47-BEF5-17303DC0469A}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="96">
   <si>
     <t>Nr.</t>
   </si>
@@ -493,6 +493,9 @@
   <si>
     <t>Distribution of Forecast / Monatsverteilung</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
 </sst>
 </file>
 
@@ -504,7 +507,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; €&quot;"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -619,6 +622,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -700,7 +709,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -773,6 +782,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -793,7 +828,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -866,6 +901,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -5527,16 +5568,16 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="O1" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{ED0F4801-55AC-584A-97BE-17C93D6D0E1F}">
+  <threadedComment ref="O10" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{E45442EF-B789-F747-94A0-67C234C866AE}">
     <text>Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</text>
   </threadedComment>
-  <threadedComment ref="Q1" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{05417129-CD48-C74E-9020-C754C6816560}">
+  <threadedComment ref="Q10" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{0E5EDB66-204F-AF48-AF0C-800703AD109B}">
     <text>gewichtete Nettosumme abzügiich bereits faktuierter Beträge</text>
   </threadedComment>
-  <threadedComment ref="X1" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{A8EB9EF4-9E59-0C48-894D-F722617BD399}">
+  <threadedComment ref="X10" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{E18BEFC3-4A25-4C4E-8456-D4AA5435172B}">
     <text>Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</text>
   </threadedComment>
-  <threadedComment ref="Y1" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{6BA95036-6D30-5548-82CC-FCCC89EFA3EF}">
+  <threadedComment ref="Y10" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{876D63B5-EF23-C74F-AFE0-495EE5563AFA}">
     <text>Das Budget ist um den angegebenen Betrag unter- (negative Werte) oder überschritten (positive Werte)</text>
   </threadedComment>
 </ThreadedComments>
@@ -5544,16 +5585,16 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="O1" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{645A51E0-CF7B-4042-B0FE-74F0618602F1}">
+  <threadedComment ref="O10" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{164688EE-C018-C74D-9C06-663D4DFF9926}">
     <text>Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</text>
   </threadedComment>
-  <threadedComment ref="Q1" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{9099E2DF-84A2-AB44-BB64-42C60828BEA6}">
+  <threadedComment ref="Q10" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{8A1ADE95-CAA9-B447-9E86-6A4505BBEEA3}">
     <text>gewichtete Nettosumme abzügiich bereits faktuierter Beträge</text>
   </threadedComment>
-  <threadedComment ref="X1" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{6F893BEE-C504-044C-9481-4570AAFDCB74}">
+  <threadedComment ref="X10" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{DDB2B422-1A98-B042-B162-FC9B5B1C5A39}">
     <text>Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</text>
   </threadedComment>
-  <threadedComment ref="Y1" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{5DE2B462-19A1-4A4E-9F4A-C3A45444414B}">
+  <threadedComment ref="Y10" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{4BF7C68F-136F-1D47-BEF5-17303DC0469A}">
     <text>Das Budget ist um den angegebenen Betrag unter- (negative Werte) oder überschritten (positive Werte)</text>
   </threadedComment>
 </ThreadedComments>
@@ -5561,7 +5602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS9"/>
+  <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
@@ -5733,8 +5774,8 @@
       </c>
     </row>
     <row r="2" spans="1:45" ht="20" x14ac:dyDescent="0.15">
-      <c r="A2" s="34">
-        <v>45658</v>
+      <c r="A2" s="34" t="s">
+        <v>95</v>
       </c>
       <c r="B2" s="34"/>
       <c r="AA2" s="6" t="s">
@@ -6160,11 +6201,145 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:45" ht="28" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="U10" s="33"/>
+      <c r="V10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X10" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y10" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN10" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR10" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS10" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="T10:U10"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6875,7 +7050,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AD000D-C6FB-164B-AFB3-9CB348DD95B6}">
-  <dimension ref="A1:AS9"/>
+  <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
@@ -6972,10 +7147,10 @@
       <c r="S1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="33"/>
+      <c r="U1" s="40"/>
       <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
@@ -7048,8 +7223,8 @@
       </c>
     </row>
     <row r="2" spans="1:45" ht="20" x14ac:dyDescent="0.15">
-      <c r="A2" s="34">
-        <v>45658</v>
+      <c r="A2" s="34" t="s">
+        <v>95</v>
       </c>
       <c r="B2" s="34"/>
       <c r="AA2" s="6" t="s">
@@ -7425,11 +7600,145 @@
     <row r="9" spans="1:45" x14ac:dyDescent="0.15">
       <c r="AA9" s="29"/>
     </row>
+    <row r="10" spans="1:45" ht="28" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="U10" s="33"/>
+      <c r="V10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X10" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y10" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN10" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR10" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS10" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="T10:U10"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
ForecastExport: filtering by unit, customer and projects is now supported (including refreshing of forecast data and graphics)
</commit_message>
<xml_diff>
--- a/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
+++ b/projectforge-business/src/main/resources/officeTemplates/ForecastTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Micromata/ProjectForge/projectforge-business/src/main/resources/officeTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DEF194-E9F3-1049-A9CA-349944543804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93D5519-0A25-A846-A4D4-47DD7A40BCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1000" windowWidth="34560" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forecast_Data" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,8 @@
   </sheets>
   <definedNames>
     <definedName name="__xlfn_SUMIFS">#N/A</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AM$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Planning_Data!$A$1:$AM$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast_Data!$A$1:$AN$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Planning_Data!$A$1:$AN$9</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -51,7 +51,7 @@
     <author>tc={876D63B5-EF23-C74F-AFE0-495EE5563AFA}</author>
   </authors>
   <commentList>
-    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{E45442EF-B789-F747-94A0-67C234C866AE}">
+    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{E45442EF-B789-F747-94A0-67C234C866AE}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -59,7 +59,7 @@
     Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</t>
       </text>
     </comment>
-    <comment ref="Q10" authorId="1" shapeId="0" xr:uid="{0E5EDB66-204F-AF48-AF0C-800703AD109B}">
+    <comment ref="R10" authorId="1" shapeId="0" xr:uid="{0E5EDB66-204F-AF48-AF0C-800703AD109B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -67,7 +67,7 @@
     gewichtete Nettosumme abzügiich bereits faktuierter Beträge</t>
       </text>
     </comment>
-    <comment ref="X10" authorId="2" shapeId="0" xr:uid="{E18BEFC3-4A25-4C4E-8456-D4AA5435172B}">
+    <comment ref="Y10" authorId="2" shapeId="0" xr:uid="{E18BEFC3-4A25-4C4E-8456-D4AA5435172B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -75,7 +75,7 @@
     Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</t>
       </text>
     </comment>
-    <comment ref="Y10" authorId="3" shapeId="0" xr:uid="{876D63B5-EF23-C74F-AFE0-495EE5563AFA}">
+    <comment ref="Z10" authorId="3" shapeId="0" xr:uid="{876D63B5-EF23-C74F-AFE0-495EE5563AFA}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -96,7 +96,7 @@
     <author>tc={4BF7C68F-136F-1D47-BEF5-17303DC0469A}</author>
   </authors>
   <commentList>
-    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{164688EE-C018-C74D-9C06-663D4DFF9926}">
+    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{164688EE-C018-C74D-9C06-663D4DFF9926}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -104,7 +104,7 @@
     Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</t>
       </text>
     </comment>
-    <comment ref="Q10" authorId="1" shapeId="0" xr:uid="{8A1ADE95-CAA9-B447-9E86-6A4505BBEEA3}">
+    <comment ref="R10" authorId="1" shapeId="0" xr:uid="{8A1ADE95-CAA9-B447-9E86-6A4505BBEEA3}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -112,7 +112,7 @@
     gewichtete Nettosumme abzügiich bereits faktuierter Beträge</t>
       </text>
     </comment>
-    <comment ref="X10" authorId="2" shapeId="0" xr:uid="{DDB2B422-1A98-B042-B162-FC9B5B1C5A39}">
+    <comment ref="Y10" authorId="2" shapeId="0" xr:uid="{DDB2B422-1A98-B042-B162-FC9B5B1C5A39}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -120,7 +120,7 @@
     Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</t>
       </text>
     </comment>
-    <comment ref="Y10" authorId="3" shapeId="0" xr:uid="{4BF7C68F-136F-1D47-BEF5-17303DC0469A}">
+    <comment ref="Z10" authorId="3" shapeId="0" xr:uid="{4BF7C68F-136F-1D47-BEF5-17303DC0469A}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="101">
   <si>
     <t>Nr.</t>
   </si>
@@ -495,6 +495,21 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>ProjectID</t>
+  </si>
+  <si>
+    <t>visibleID</t>
+  </si>
+  <si>
+    <t>unused</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -822,7 +837,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -877,6 +892,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1133,7 +1154,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$2:$AM$2</c:f>
+              <c:f>Forecast_Data!$AC$2:$AN$2</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1222,7 +1243,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$4:$AM$4</c:f>
+              <c:f>Forecast_Data!$AC$4:$AN$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1311,7 +1332,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$3:$AM$3</c:f>
+              <c:f>Forecast_Data!$AC$3:$AN$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1400,7 +1421,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$6:$AM$6</c:f>
+              <c:f>Forecast_Data!$AC$6:$AN$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1491,7 +1512,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$5:$AM$5</c:f>
+              <c:f>Forecast_Data!$AC$5:$AN$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1566,7 +1587,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$8:$AM$8</c:f>
+              <c:f>Forecast_Data!$AC$8:$AN$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1636,7 +1657,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Forecast_Data!$AA$9</c:f>
+              <c:f>Forecast_Data!$AB$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1665,7 +1686,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Forecast_Data!$AB$1:$AM$1</c:f>
+              <c:f>Forecast_Data!$AC$1:$AN$1</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1709,7 +1730,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$9:$AM$9</c:f>
+              <c:f>Forecast_Data!$AC$9:$AN$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3079,7 +3100,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Forecast_Data!$AA$9</c:f>
+              <c:f>Forecast_Data!$AB$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3111,7 +3132,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Forecast_Data!$AB$9:$AM$9</c:f>
+              <c:f>Forecast_Data!$AC$9:$AN$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5562,16 +5583,16 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="O10" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{E45442EF-B789-F747-94A0-67C234C866AE}">
+  <threadedComment ref="P10" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{E45442EF-B789-F747-94A0-67C234C866AE}">
     <text>Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</text>
   </threadedComment>
-  <threadedComment ref="Q10" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{0E5EDB66-204F-AF48-AF0C-800703AD109B}">
+  <threadedComment ref="R10" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{0E5EDB66-204F-AF48-AF0C-800703AD109B}">
     <text>gewichtete Nettosumme abzügiich bereits faktuierter Beträge</text>
   </threadedComment>
-  <threadedComment ref="X10" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{E18BEFC3-4A25-4C4E-8456-D4AA5435172B}">
+  <threadedComment ref="Y10" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{E18BEFC3-4A25-4C4E-8456-D4AA5435172B}">
     <text>Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</text>
   </threadedComment>
-  <threadedComment ref="Y10" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{876D63B5-EF23-C74F-AFE0-495EE5563AFA}">
+  <threadedComment ref="Z10" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{876D63B5-EF23-C74F-AFE0-495EE5563AFA}">
     <text>Das Budget ist um den angegebenen Betrag unter- (negative Werte) oder überschritten (positive Werte)</text>
   </threadedComment>
 </ThreadedComments>
@@ -5579,16 +5600,16 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="O10" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{164688EE-C018-C74D-9C06-663D4DFF9926}">
+  <threadedComment ref="P10" dT="2019-12-19T15:09:32.91" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{164688EE-C018-C74D-9C06-663D4DFF9926}">
     <text>Nettosumme gewichtet mit der Eintrittswahrscheinlichkeit</text>
   </threadedComment>
-  <threadedComment ref="Q10" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{8A1ADE95-CAA9-B447-9E86-6A4505BBEEA3}">
+  <threadedComment ref="R10" dT="2019-12-19T15:10:08.52" personId="{33547D16-133A-3948-B40B-5CD925F3958C}" id="{8A1ADE95-CAA9-B447-9E86-6A4505BBEEA3}">
     <text>gewichtete Nettosumme abzügiich bereits faktuierter Beträge</text>
   </threadedComment>
-  <threadedComment ref="X10" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{DDB2B422-1A98-B042-B162-FC9B5B1C5A39}">
+  <threadedComment ref="Y10" dT="2025-01-09T14:32:39.85" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{DDB2B422-1A98-B042-B162-FC9B5B1C5A39}">
     <text>Diese Beträge sind nach dem betrachteten Forecast-Zeitraum noch offen. Werden demnach später in Rechnung gestellt.</text>
   </threadedComment>
-  <threadedComment ref="Y10" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{4BF7C68F-136F-1D47-BEF5-17303DC0469A}">
+  <threadedComment ref="Z10" dT="2025-01-09T14:33:25.24" personId="{A78CCFA2-D802-6742-9423-F4345C0EED1C}" id="{4BF7C68F-136F-1D47-BEF5-17303DC0469A}">
     <text>Das Budget ist um den angegebenen Betrag unter- (negative Werte) oder überschritten (positive Werte)</text>
   </threadedComment>
 </ThreadedComments>
@@ -5596,744 +5617,773 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS10"/>
+  <dimension ref="A1:AW10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="10" topLeftCell="W11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="10" topLeftCell="X11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="AB9" sqref="AB9"/>
+      <selection pane="bottomRight" activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="7" width="31.1640625" customWidth="1"/>
-    <col min="8" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="2" customWidth="1"/>
-    <col min="16" max="18" width="11.5" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="20" customWidth="1"/>
-    <col min="20" max="21" width="11.5" style="1" customWidth="1"/>
-    <col min="22" max="23" width="8" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" style="25" customWidth="1"/>
-    <col min="25" max="25" width="13.1640625" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.5" customWidth="1"/>
-    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="39" width="12.83203125" style="2" customWidth="1"/>
-    <col min="40" max="41" width="19" style="1" customWidth="1"/>
-    <col min="42" max="42" width="52.83203125" customWidth="1"/>
-    <col min="43" max="43" width="16.5" customWidth="1"/>
-    <col min="44" max="44" width="29.5" customWidth="1"/>
-    <col min="45" max="45" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="8" width="31.1640625" customWidth="1"/>
+    <col min="9" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="2" customWidth="1"/>
+    <col min="17" max="19" width="11.5" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.5" style="20" customWidth="1"/>
+    <col min="21" max="22" width="11.5" style="1" customWidth="1"/>
+    <col min="23" max="24" width="8" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" style="25" customWidth="1"/>
+    <col min="26" max="26" width="13.1640625" style="25" customWidth="1"/>
+    <col min="27" max="27" width="11.5" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="40" width="12.83203125" style="2" customWidth="1"/>
+    <col min="41" max="42" width="19" style="1" customWidth="1"/>
+    <col min="43" max="43" width="52.83203125" customWidth="1"/>
+    <col min="44" max="44" width="16.5" customWidth="1"/>
+    <col min="45" max="45" width="29.5" customWidth="1"/>
+    <col min="46" max="46" width="65.6640625" customWidth="1"/>
+    <col min="47" max="47" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="9.5" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="10.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:49" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="U1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="35"/>
+      <c r="W1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="22" t="s">
+      <c r="AO1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AO1" s="22" t="s">
+      <c r="AP1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AP1" s="26" t="s">
+      <c r="AQ1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AS1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="AU1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW1" s="33" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="2" spans="1:45" ht="20" x14ac:dyDescent="0.15">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:49" ht="20" x14ac:dyDescent="0.15">
+      <c r="A2" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="AA2" s="6" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="34"/>
+      <c r="AB2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="7">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=beauftragt")</f>
-        <v>0</v>
-      </c>
       <c r="AC2" s="7">
-        <f t="shared" ref="AC2:AM2" si="0">SUMIFS(AC11:AC65537,$K11:$K65537,"=beauftragt")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=beauftragt",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AD2:AN2" ca="1" si="0">SUMIFS(AD11:AD100000,$L11:$L100000,"=beauftragt",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AE2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AF2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AG2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AH2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AI2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AK2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AL2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AM2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN2" s="7">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA3" s="8" t="s">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="9">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=gelegt")</f>
-        <v>0</v>
-      </c>
       <c r="AC3" s="9">
-        <f t="shared" ref="AC3:AM3" si="1">SUMIFS(AC11:AC65537,$K11:$K65537,"=gelegt")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=gelegt",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AD3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AD3:AN3" ca="1" si="1">SUMIFS(AD11:AD100000,$L11:$L100000,"=gelegt",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AE3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AF3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AG3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AH3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AI3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AK3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AL3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AM3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN3" s="9">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA4" s="6" t="s">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AB4" s="7">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=LOI")</f>
-        <v>0</v>
-      </c>
       <c r="AC4" s="7">
-        <f t="shared" ref="AC4:AM4" si="2">SUMIFS(AC11:AC65537,$K11:$K65537,"=LOI")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=LOI",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AD4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AD4:AN4" ca="1" si="2">SUMIFS(AD11:AD100000,$L11:$L100000,"=LOI",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AE4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AF4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AG4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AH4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AI4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AK4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AL4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AM4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN4" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA5" s="8" t="s">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="9">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=in Erstellung")</f>
-        <v>0</v>
-      </c>
       <c r="AC5" s="9">
-        <f t="shared" ref="AC5:AM5" si="3">SUMIFS(AC11:AC65537,$K11:$K65537,"=in Erstellung")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=in Erstellung",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AD5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AD5:AN5" ca="1" si="3">SUMIFS(AD11:AD100000,$L11:$L100000,"=in Erstellung",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AE5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AF5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AG5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AH5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AI5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AK5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AL5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AM5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN5" s="9">
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA6" s="10" t="s">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AB6" s="11">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=Potenzial")</f>
-        <v>0</v>
-      </c>
       <c r="AC6" s="11">
-        <f t="shared" ref="AC6:AM6" si="4">SUMIFS(AC11:AC65537,$K11:$K65537,"=Potenzial")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=Potenzial",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AD6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AD6:AN6" ca="1" si="4">SUMIFS(AD11:AD100000,$L11:$L100000,"=Potenzial",$AV11:$AV100000,1)</f>
         <v>0</v>
       </c>
       <c r="AE6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AF6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AG6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AH6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AI6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AK6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AL6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AM6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AN6" s="11">
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA7" s="12" t="s">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AB7" s="9">
-        <f t="shared" ref="AB7:AM7" si="5">SUM(AB2:AB6)</f>
-        <v>0</v>
-      </c>
       <c r="AC7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AC7:AN7" ca="1" si="5">SUM(AC2:AC6)</f>
         <v>0</v>
       </c>
       <c r="AD7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AE7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AF7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AG7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AH7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AI7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AK7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AL7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AM7" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AN7" s="9">
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA8" s="13" t="s">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AB8" s="14">
-        <f>SUM(Rechnungen!M2:M65535)</f>
-        <v>0</v>
-      </c>
       <c r="AC8" s="14">
-        <f>SUM(Rechnungen!N2:N65535)</f>
+        <f>SUMIFS(Rechnungen!M:M, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AD8" s="14">
-        <f>SUM(Rechnungen!O2:O65535)</f>
+        <f>SUMIFS(Rechnungen!N:N, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AE8" s="14">
-        <f>SUM(Rechnungen!P2:P65535)</f>
+        <f>SUMIFS(Rechnungen!O:O, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AF8" s="14">
-        <f>SUM(Rechnungen!Q2:Q65535)</f>
+        <f>SUMIFS(Rechnungen!P:P, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AG8" s="14">
-        <f>SUM(Rechnungen!R2:R65535)</f>
+        <f>SUMIFS(Rechnungen!Q:Q, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AH8" s="14">
-        <f>SUM(Rechnungen!S2:S65535)</f>
+        <f>SUMIFS(Rechnungen!R:R, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AI8" s="14">
-        <f>SUM(Rechnungen!T2:T65535)</f>
+        <f>SUMIFS(Rechnungen!S:S, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AJ8" s="14">
-        <f>SUM(Rechnungen!U2:U65535)</f>
+        <f>SUMIFS(Rechnungen!T:T, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AK8" s="14">
-        <f>SUM(Rechnungen!V2:V65535)</f>
+        <f>SUMIFS(Rechnungen!U:U, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AL8" s="14">
-        <f>SUM(Rechnungen!W2:W65535)</f>
+        <f>SUMIFS(Rechnungen!V:V, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AM8" s="14">
-        <f>SUM(Rechnungen!X2:X65535)</f>
+        <f>SUMIFS(Rechnungen!W:W, Rechnungen!$Z:$Z, TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="AN8" s="14">
+        <f>SUMIFS(Rechnungen!X:X, Rechnungen!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA9" s="15" t="s">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AB9" s="16">
-        <f>Planning_Data!AB7</f>
-        <v>0</v>
-      </c>
       <c r="AC9" s="16">
-        <f>Planning_Data!AC7</f>
+        <f ca="1">Planning_Data!AC7</f>
         <v>0</v>
       </c>
       <c r="AD9" s="16">
-        <f>Planning_Data!AD7</f>
+        <f ca="1">Planning_Data!AD7</f>
         <v>0</v>
       </c>
       <c r="AE9" s="16">
-        <f>Planning_Data!AE7</f>
+        <f ca="1">Planning_Data!AE7</f>
         <v>0</v>
       </c>
       <c r="AF9" s="16">
-        <f>Planning_Data!AF7</f>
+        <f ca="1">Planning_Data!AF7</f>
         <v>0</v>
       </c>
       <c r="AG9" s="16">
-        <f>Planning_Data!AG7</f>
+        <f ca="1">Planning_Data!AG7</f>
         <v>0</v>
       </c>
       <c r="AH9" s="16">
-        <f>Planning_Data!AH7</f>
+        <f ca="1">Planning_Data!AH7</f>
         <v>0</v>
       </c>
       <c r="AI9" s="16">
-        <f>Planning_Data!AI7</f>
+        <f ca="1">Planning_Data!AI7</f>
         <v>0</v>
       </c>
       <c r="AJ9" s="16">
-        <f>Planning_Data!AJ7</f>
+        <f ca="1">Planning_Data!AJ7</f>
         <v>0</v>
       </c>
       <c r="AK9" s="16">
-        <f>Planning_Data!AK7</f>
+        <f ca="1">Planning_Data!AK7</f>
         <v>0</v>
       </c>
       <c r="AL9" s="16">
-        <f>Planning_Data!AL7</f>
+        <f ca="1">Planning_Data!AL7</f>
         <v>0</v>
       </c>
       <c r="AM9" s="16">
-        <f>Planning_Data!AM7</f>
+        <f ca="1">Planning_Data!AM7</f>
+        <v>0</v>
+      </c>
+      <c r="AN9" s="16">
+        <f ca="1">Planning_Data!AN7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:45" ht="28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:49" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="F10" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="G10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="H10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="K10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="R10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T10" s="33" t="s">
+      <c r="U10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="U10" s="33"/>
-      <c r="V10" s="3" t="s">
+      <c r="V10" s="35"/>
+      <c r="W10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W10" s="3" t="s">
+      <c r="X10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="X10" s="27" t="s">
+      <c r="Y10" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Y10" s="27" t="s">
+      <c r="Z10" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AA10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="5" t="s">
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AC10" s="5" t="s">
+      <c r="AD10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AD10" s="5" t="s">
+      <c r="AE10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AE10" s="5" t="s">
+      <c r="AF10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AF10" s="5" t="s">
+      <c r="AG10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AG10" s="5" t="s">
+      <c r="AH10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AH10" s="5" t="s">
+      <c r="AI10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AI10" s="5" t="s">
+      <c r="AJ10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AJ10" s="5" t="s">
+      <c r="AK10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AK10" s="5" t="s">
+      <c r="AL10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AL10" s="5" t="s">
+      <c r="AM10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AM10" s="5" t="s">
+      <c r="AN10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AN10" s="22" t="s">
+      <c r="AO10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AO10" s="22" t="s">
+      <c r="AP10" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AP10" s="26" t="s">
+      <c r="AQ10" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AQ10" s="21" t="s">
+      <c r="AR10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AR10" s="21" t="s">
+      <c r="AS10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AS10" s="21" t="s">
+      <c r="AT10" s="21" t="s">
         <v>18</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW10" s="33" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="3">
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="U1:V1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="U10:V10"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6392,7 +6442,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6403,51 +6453,51 @@
   <sheetData>
     <row r="1" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B1" s="23" t="str">
-        <f>Forecast_Data!AB1</f>
+        <f>Forecast_Data!AC1</f>
         <v>Month 1</v>
       </c>
       <c r="C1" s="23" t="str">
-        <f>Forecast_Data!AC1</f>
+        <f>Forecast_Data!AD1</f>
         <v>Month 2</v>
       </c>
       <c r="D1" s="23" t="str">
-        <f>Forecast_Data!AD1</f>
+        <f>Forecast_Data!AE1</f>
         <v>Month 3</v>
       </c>
       <c r="E1" s="23" t="str">
-        <f>Forecast_Data!AE1</f>
+        <f>Forecast_Data!AF1</f>
         <v>Month 4</v>
       </c>
       <c r="F1" s="23" t="str">
-        <f>Forecast_Data!AF1</f>
+        <f>Forecast_Data!AG1</f>
         <v>Month 5</v>
       </c>
       <c r="G1" s="23" t="str">
-        <f>Forecast_Data!AG1</f>
+        <f>Forecast_Data!AH1</f>
         <v>Month 6</v>
       </c>
       <c r="H1" s="23" t="str">
-        <f>Forecast_Data!AH1</f>
+        <f>Forecast_Data!AI1</f>
         <v>Month 7</v>
       </c>
       <c r="I1" s="23" t="str">
-        <f>Forecast_Data!AI1</f>
+        <f>Forecast_Data!AJ1</f>
         <v>Month 8</v>
       </c>
       <c r="J1" s="23" t="str">
-        <f>Forecast_Data!AJ1</f>
+        <f>Forecast_Data!AK1</f>
         <v>Month 9</v>
       </c>
       <c r="K1" s="23" t="str">
-        <f>Forecast_Data!AK1</f>
+        <f>Forecast_Data!AL1</f>
         <v>Month 10</v>
       </c>
       <c r="L1" s="23" t="str">
-        <f>Forecast_Data!AL1</f>
+        <f>Forecast_Data!AM1</f>
         <v>Month 11</v>
       </c>
       <c r="M1" s="23" t="str">
-        <f>Forecast_Data!AM1</f>
+        <f>Forecast_Data!AN1</f>
         <v>Month 12</v>
       </c>
     </row>
@@ -6456,51 +6506,51 @@
         <v>25</v>
       </c>
       <c r="B2" s="17">
-        <f>Forecast_Data!AB8</f>
+        <f>Forecast_Data!AC8</f>
         <v>0</v>
       </c>
       <c r="C2" s="17">
-        <f>Forecast_Data!AC8</f>
+        <f>Forecast_Data!AD8</f>
         <v>0</v>
       </c>
       <c r="D2" s="17">
-        <f>Forecast_Data!AD8</f>
+        <f>Forecast_Data!AE8</f>
         <v>0</v>
       </c>
       <c r="E2" s="17">
-        <f>Forecast_Data!AE8</f>
+        <f>Forecast_Data!AF8</f>
         <v>0</v>
       </c>
       <c r="F2" s="17">
-        <f>Forecast_Data!AF8</f>
+        <f>Forecast_Data!AG8</f>
         <v>0</v>
       </c>
       <c r="G2" s="17">
-        <f>Forecast_Data!AG8</f>
+        <f>Forecast_Data!AH8</f>
         <v>0</v>
       </c>
       <c r="H2" s="17">
-        <f>Forecast_Data!AH8</f>
+        <f>Forecast_Data!AI8</f>
         <v>0</v>
       </c>
       <c r="I2" s="17">
-        <f>Forecast_Data!AI8</f>
+        <f>Forecast_Data!AJ8</f>
         <v>0</v>
       </c>
       <c r="J2" s="17">
-        <f>Forecast_Data!AJ8</f>
+        <f>Forecast_Data!AK8</f>
         <v>0</v>
       </c>
       <c r="K2" s="17">
-        <f>Forecast_Data!AK8</f>
+        <f>Forecast_Data!AL8</f>
         <v>0</v>
       </c>
       <c r="L2" s="17">
-        <f>Forecast_Data!AL8</f>
+        <f>Forecast_Data!AM8</f>
         <v>0</v>
       </c>
       <c r="M2" s="17">
-        <f>Forecast_Data!AM8</f>
+        <f>Forecast_Data!AN8</f>
         <v>0</v>
       </c>
     </row>
@@ -6509,51 +6559,51 @@
         <v>24</v>
       </c>
       <c r="B3" s="18">
-        <f>Forecast_Data!AB7</f>
+        <f ca="1">Forecast_Data!AC7</f>
         <v>0</v>
       </c>
       <c r="C3" s="18">
-        <f>Forecast_Data!AC7</f>
+        <f ca="1">Forecast_Data!AD7</f>
         <v>0</v>
       </c>
       <c r="D3" s="18">
-        <f>Forecast_Data!AD7</f>
+        <f ca="1">Forecast_Data!AE7</f>
         <v>0</v>
       </c>
       <c r="E3" s="18">
-        <f>Forecast_Data!AE7</f>
+        <f ca="1">Forecast_Data!AF7</f>
         <v>0</v>
       </c>
       <c r="F3" s="18">
-        <f>Forecast_Data!AF7</f>
+        <f ca="1">Forecast_Data!AG7</f>
         <v>0</v>
       </c>
       <c r="G3" s="18">
-        <f>Forecast_Data!AG7</f>
+        <f ca="1">Forecast_Data!AH7</f>
         <v>0</v>
       </c>
       <c r="H3" s="18">
-        <f>Forecast_Data!AH7</f>
+        <f ca="1">Forecast_Data!AI7</f>
         <v>0</v>
       </c>
       <c r="I3" s="18">
-        <f>Forecast_Data!AI7</f>
+        <f ca="1">Forecast_Data!AJ7</f>
         <v>0</v>
       </c>
       <c r="J3" s="18">
-        <f>Forecast_Data!AJ7</f>
+        <f ca="1">Forecast_Data!AK7</f>
         <v>0</v>
       </c>
       <c r="K3" s="18">
-        <f>Forecast_Data!AK7</f>
+        <f ca="1">Forecast_Data!AL7</f>
         <v>0</v>
       </c>
       <c r="L3" s="18">
-        <f>Forecast_Data!AL7</f>
+        <f ca="1">Forecast_Data!AM7</f>
         <v>0</v>
       </c>
       <c r="M3" s="18">
-        <f>Forecast_Data!AM7</f>
+        <f ca="1">Forecast_Data!AN7</f>
         <v>0</v>
       </c>
     </row>
@@ -6562,51 +6612,51 @@
         <v>27</v>
       </c>
       <c r="B4" s="18">
-        <f>MAX(B2,B3)</f>
+        <f ca="1">MAX(B2,B3)</f>
         <v>0</v>
       </c>
       <c r="C4" s="18">
-        <f t="shared" ref="C4:M4" si="0">MAX(C2,C3)</f>
+        <f t="shared" ref="C4:M4" ca="1" si="0">MAX(C2,C3)</f>
         <v>0</v>
       </c>
       <c r="D4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="F4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="G4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="I4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="K4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="L4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="M4" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6615,51 +6665,51 @@
         <v>28</v>
       </c>
       <c r="B5" s="19">
-        <f>B4</f>
+        <f ca="1">B4</f>
         <v>0</v>
       </c>
       <c r="C5" s="19">
-        <f>B5+C4</f>
+        <f ca="1">B5+C4</f>
         <v>0</v>
       </c>
       <c r="D5" s="19">
-        <f t="shared" ref="D5:M5" si="1">C5+D4</f>
+        <f t="shared" ref="D5:M5" ca="1" si="1">C5+D4</f>
         <v>0</v>
       </c>
       <c r="E5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="F5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="G5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="H5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="K5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="L5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="M5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6668,51 +6718,51 @@
         <v>29</v>
       </c>
       <c r="B6" s="19">
-        <f>Forecast_Data!AB9</f>
+        <f ca="1">Forecast_Data!AC9</f>
         <v>0</v>
       </c>
       <c r="C6" s="19">
-        <f>B6+Forecast_Data!AC9</f>
+        <f ca="1">B6+Forecast_Data!AD9</f>
         <v>0</v>
       </c>
       <c r="D6" s="19">
-        <f>C6+Forecast_Data!AD9</f>
+        <f ca="1">C6+Forecast_Data!AE9</f>
         <v>0</v>
       </c>
       <c r="E6" s="19">
-        <f>D6+Forecast_Data!AE9</f>
+        <f ca="1">D6+Forecast_Data!AF9</f>
         <v>0</v>
       </c>
       <c r="F6" s="19">
-        <f>E6+Forecast_Data!AF9</f>
+        <f ca="1">E6+Forecast_Data!AG9</f>
         <v>0</v>
       </c>
       <c r="G6" s="19">
-        <f>F6+Forecast_Data!AG9</f>
+        <f ca="1">F6+Forecast_Data!AH9</f>
         <v>0</v>
       </c>
       <c r="H6" s="19">
-        <f>G6+Forecast_Data!AH9</f>
+        <f ca="1">G6+Forecast_Data!AI9</f>
         <v>0</v>
       </c>
       <c r="I6" s="19">
-        <f>H6+Forecast_Data!AI9</f>
+        <f ca="1">H6+Forecast_Data!AJ9</f>
         <v>0</v>
       </c>
       <c r="J6" s="19">
-        <f>I6+Forecast_Data!AJ9</f>
+        <f ca="1">I6+Forecast_Data!AK9</f>
         <v>0</v>
       </c>
       <c r="K6" s="19">
-        <f>J6+Forecast_Data!AK9</f>
+        <f ca="1">J6+Forecast_Data!AL9</f>
         <v>0</v>
       </c>
       <c r="L6" s="19">
-        <f>K6+Forecast_Data!AL9</f>
+        <f ca="1">K6+Forecast_Data!AM9</f>
         <v>0</v>
       </c>
       <c r="M6" s="19">
-        <f>L6+Forecast_Data!AM9</f>
+        <f ca="1">L6+Forecast_Data!AN9</f>
         <v>0</v>
       </c>
     </row>
@@ -6734,51 +6784,51 @@
         <v>52</v>
       </c>
       <c r="B8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!M2:M65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!M:M, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="C8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!N2:N65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!N:N, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="D8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!O2:O65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!O:O, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="E8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!P2:P65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!P:P, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="F8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!Q2:Q65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!Q:Q, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="G8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!R2:R65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!R:R, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="H8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!S2:S65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!S:S, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="I8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!T2:T65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!T:T, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="J8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!U2:U65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!U:U, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="K8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!V2:V65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!V:V, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="L8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!W2:W65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!W:W, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="M8" s="19">
-        <f>SUM('Rechnungen Vorjahr'!X2:X65534)</f>
+        <f>SUMIFS('Rechnungen Vorjahr'!X:X, 'Rechnungen Vorjahr'!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
     </row>
@@ -6845,13 +6895,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007BFD20-C3FD-B945-8889-0EABEB8C212C}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6860,9 +6910,10 @@
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="6" max="6" width="18.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -6887,10 +6938,10 @@
       <c r="H1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="35"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="13" t="s">
         <v>50</v>
       </c>
@@ -6932,6 +6983,12 @@
       </c>
       <c r="X1" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -6945,13 +7002,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477A8465-810E-0B43-A1C7-F27798459BF0}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6960,9 +7017,10 @@
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="6" max="6" width="18.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -6987,10 +7045,10 @@
       <c r="H1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="35"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="13" t="s">
         <v>50</v>
       </c>
@@ -7032,6 +7090,12 @@
       </c>
       <c r="X1" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -7044,695 +7108,721 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AD000D-C6FB-164B-AFB3-9CB348DD95B6}">
-  <dimension ref="A1:AS10"/>
+  <dimension ref="A1:AW10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="10" topLeftCell="W11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="10" topLeftCell="X12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="AB11" sqref="AB11"/>
+      <selection pane="bottomRight" activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="7" width="31.1640625" customWidth="1"/>
-    <col min="8" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.5" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="2" customWidth="1"/>
-    <col min="16" max="18" width="11.5" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="20" customWidth="1"/>
-    <col min="20" max="21" width="11.5" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8" customWidth="1"/>
-    <col min="23" max="23" width="8.33203125" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" style="25" customWidth="1"/>
-    <col min="25" max="25" width="13.1640625" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.5" customWidth="1"/>
-    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="39" width="12.83203125" style="2" customWidth="1"/>
-    <col min="40" max="41" width="19" style="1" customWidth="1"/>
-    <col min="42" max="42" width="52.83203125" customWidth="1"/>
-    <col min="43" max="43" width="16.5" customWidth="1"/>
-    <col min="44" max="44" width="29.5" customWidth="1"/>
-    <col min="45" max="45" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="8" width="31.1640625" customWidth="1"/>
+    <col min="9" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="2" customWidth="1"/>
+    <col min="17" max="19" width="11.5" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.5" style="20" customWidth="1"/>
+    <col min="21" max="22" width="11.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="8" customWidth="1"/>
+    <col min="24" max="24" width="8.33203125" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" style="25" customWidth="1"/>
+    <col min="26" max="26" width="13.1640625" style="25" customWidth="1"/>
+    <col min="27" max="27" width="11.5" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="40" width="12.83203125" style="2" customWidth="1"/>
+    <col min="41" max="42" width="19" style="1" customWidth="1"/>
+    <col min="43" max="43" width="52.83203125" customWidth="1"/>
+    <col min="44" max="44" width="16.5" customWidth="1"/>
+    <col min="45" max="45" width="29.5" customWidth="1"/>
+    <col min="46" max="46" width="65.6640625" customWidth="1"/>
+    <col min="47" max="47" width="9.6640625" customWidth="1"/>
+    <col min="48" max="48" width="8.33203125" customWidth="1"/>
+    <col min="49" max="49" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:49" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="U1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="37"/>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="39"/>
+      <c r="W1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="22" t="s">
+      <c r="AO1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AO1" s="22" t="s">
+      <c r="AP1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AP1" s="26" t="s">
+      <c r="AQ1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AS1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="AU1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW1" s="33" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="2" spans="1:45" ht="20" x14ac:dyDescent="0.15">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:49" ht="20" x14ac:dyDescent="0.15">
+      <c r="A2" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="AA2" s="6" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="34"/>
+      <c r="AB2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="7">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=beauftragt")</f>
-        <v>0</v>
-      </c>
       <c r="AC2" s="7">
-        <f t="shared" ref="AC2:AM2" si="0">SUMIFS(AC11:AC65537,$K11:$K65537,"=beauftragt")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=beauftragt",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AD2:AN2" ca="1" si="0">SUMIFS(AD11:AD100000,$L11:$L100000,"=beauftragt",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AE2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AF2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AG2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AH2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AI2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AK2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AL2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AM2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN2" s="7">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA3" s="8" t="s">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="9">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=gelegt")</f>
-        <v>0</v>
-      </c>
       <c r="AC3" s="9">
-        <f t="shared" ref="AC3:AM3" si="1">SUMIFS(AC11:AC65537,$K11:$K65537,"=gelegt")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=gelegt",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AD3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AD3:AN3" ca="1" si="1">SUMIFS(AD11:AD100000,$L11:$L100000,"=gelegt",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AE3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AF3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AG3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AH3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AI3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AK3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AL3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="AM3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN3" s="9">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA4" s="6" t="s">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AB4" s="7">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=LOI")</f>
-        <v>0</v>
-      </c>
       <c r="AC4" s="7">
-        <f t="shared" ref="AC4:AM4" si="2">SUMIFS(AC11:AC65537,$K11:$K65537,"=LOI")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=LOI",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AD4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AD4:AN4" ca="1" si="2">SUMIFS(AD11:AD100000,$L11:$L100000,"=LOI",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AE4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AF4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AG4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AH4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AI4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AK4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AL4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AM4" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN4" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA5" s="8" t="s">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="9">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=in Erstellung")</f>
-        <v>0</v>
-      </c>
       <c r="AC5" s="9">
-        <f t="shared" ref="AC5:AM5" si="3">SUMIFS(AC11:AC65537,$K11:$K65537,"=in Erstellung")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=in Erstellung",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AD5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AD5:AN5" ca="1" si="3">SUMIFS(AD11:AD100000,$L11:$L100000,"=in Erstellung",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AE5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AF5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AG5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AH5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AI5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AK5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AL5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AM5" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN5" s="9">
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA6" s="10" t="s">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AB6" s="11">
-        <f>SUMIFS(AB11:AB65537,$K11:$K65537,"=Potenzial")</f>
-        <v>0</v>
-      </c>
       <c r="AC6" s="11">
-        <f t="shared" ref="AC6:AM6" si="4">SUMIFS(AC11:AC65537,$K11:$K65537,"=Potenzial")</f>
+        <f ca="1">SUMIFS(AC11:AC100000,$L11:$L100000,"=Potenzial",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AD6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AD6:AN6" ca="1" si="4">SUMIFS(AD11:AD100000,$L11:$L100000,"=Potenzial",$AV11:$AV100000, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AE6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AF6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AG6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AH6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AI6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AK6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AL6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AM6" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AN6" s="11">
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA7" s="15" t="s">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AB7" s="16">
-        <f>MAX(SUM(AB2:AB6),AB8)</f>
-        <v>0</v>
-      </c>
       <c r="AC7" s="16">
-        <f t="shared" ref="AC7:AM7" si="5">MAX(SUM(AC2:AC6),AC8)</f>
+        <f ca="1">MAX(SUM(AC2:AC6),AC8)</f>
         <v>0</v>
       </c>
       <c r="AD7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AD7:AN7" ca="1" si="5">MAX(SUM(AD2:AD6),AD8)</f>
         <v>0</v>
       </c>
       <c r="AE7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AF7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AG7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AH7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AI7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AK7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AL7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="AM7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AN7" s="16">
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA8" s="13" t="s">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AB8" s="14">
-        <f>SUM(Planning_Invoices!M2:M65535)</f>
-        <v>0</v>
-      </c>
       <c r="AC8" s="14">
-        <f>SUM(Planning_Invoices!N2:N65535)</f>
+        <f>SUMIFS(Planning_Invoices!M:M, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AD8" s="14">
-        <f>SUM(Planning_Invoices!O2:O65535)</f>
+        <f>SUMIFS(Planning_Invoices!N:N, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AE8" s="14">
-        <f>SUM(Planning_Invoices!P2:P65535)</f>
+        <f>SUMIFS(Planning_Invoices!O:O, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AF8" s="14">
-        <f>SUM(Planning_Invoices!Q2:Q65535)</f>
+        <f>SUMIFS(Planning_Invoices!P:P, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AG8" s="14">
-        <f>SUM(Planning_Invoices!R2:R65535)</f>
+        <f>SUMIFS(Planning_Invoices!Q:Q, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AH8" s="14">
-        <f>SUM(Planning_Invoices!S2:S65535)</f>
+        <f>SUMIFS(Planning_Invoices!R:R, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AI8" s="14">
-        <f>SUM(Planning_Invoices!T2:T65535)</f>
+        <f>SUMIFS(Planning_Invoices!S:S, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AJ8" s="14">
-        <f>SUM(Planning_Invoices!U2:U65535)</f>
+        <f>SUMIFS(Planning_Invoices!T:T, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AK8" s="14">
-        <f>SUM(Planning_Invoices!V2:V65535)</f>
+        <f>SUMIFS(Planning_Invoices!U:U, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AL8" s="14">
-        <f>SUM(Planning_Invoices!W2:W65535)</f>
+        <f>SUMIFS(Planning_Invoices!V:V, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
       <c r="AM8" s="14">
-        <f>SUM(Planning_Invoices!X2:X65535)</f>
+        <f>SUMIFS(Planning_Invoices!W:W, Planning_Invoices!$Z:$Z, TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="AN8" s="14">
+        <f>SUMIFS(Planning_Invoices!X:X, Planning_Invoices!$Z:$Z, TRUE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="AA9" s="29"/>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.15">
+      <c r="AB9" s="29"/>
     </row>
-    <row r="10" spans="1:45" ht="28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:49" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="F10" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="G10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="H10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="K10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="R10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T10" s="33" t="s">
+      <c r="U10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="U10" s="33"/>
-      <c r="V10" s="3" t="s">
+      <c r="V10" s="35"/>
+      <c r="W10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W10" s="3" t="s">
+      <c r="X10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="X10" s="27" t="s">
+      <c r="Y10" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Y10" s="27" t="s">
+      <c r="Z10" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AA10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="5" t="s">
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AC10" s="5" t="s">
+      <c r="AD10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AD10" s="5" t="s">
+      <c r="AE10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AE10" s="5" t="s">
+      <c r="AF10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AF10" s="5" t="s">
+      <c r="AG10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AG10" s="5" t="s">
+      <c r="AH10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AH10" s="5" t="s">
+      <c r="AI10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AI10" s="5" t="s">
+      <c r="AJ10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AJ10" s="5" t="s">
+      <c r="AK10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AK10" s="5" t="s">
+      <c r="AL10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AL10" s="5" t="s">
+      <c r="AM10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AM10" s="5" t="s">
+      <c r="AN10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AN10" s="22" t="s">
+      <c r="AO10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AO10" s="22" t="s">
+      <c r="AP10" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="AP10" s="26" t="s">
+      <c r="AQ10" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AQ10" s="21" t="s">
+      <c r="AR10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AR10" s="21" t="s">
+      <c r="AS10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AS10" s="21" t="s">
+      <c r="AT10" s="21" t="s">
         <v>18</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="3">
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="U1:V1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="U10:V10"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7743,13 +7833,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCC10A8-3156-B545-A437-09CFA0CFA594}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7758,9 +7848,10 @@
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="6" max="6" width="18.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -7785,10 +7876,10 @@
       <c r="H1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="35"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="13" t="s">
         <v>50</v>
       </c>
@@ -7830,6 +7921,12 @@
       </c>
       <c r="X1" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -7875,36 +7972,36 @@
       <c r="B3" s="31"/>
     </row>
     <row r="5" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="8" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">

</xml_diff>